<commit_message>
Modificado proforma y Catalogo Clientes
</commit_message>
<xml_diff>
--- a/clientes/files/TODITICO_CATÁLOGO.xlsx
+++ b/clientes/files/TODITICO_CATÁLOGO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\Documents\Catálogos Proformas\Este\400\Clientes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\Documents\Catálogos Proformas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1D5DFB-4981-45D9-B6DE-975951B25207}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42636F3-92F6-4AAD-972E-1D59CA61DF2D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="526">
   <si>
     <t>DESCRIPCION</t>
   </si>
@@ -926,9 +926,6 @@
     <t>CREMALLERAS DE PUERTAS C/U</t>
   </si>
   <si>
-    <t>CUBO DE RUEDAS</t>
-  </si>
-  <si>
     <t>CULEBRA CUENTAMILLAS</t>
   </si>
   <si>
@@ -1575,6 +1572,87 @@
   </si>
   <si>
     <t>BATERIAS 40 Ah</t>
+  </si>
+  <si>
+    <t>CUBOS DE RUEDAS PAREJA</t>
+  </si>
+  <si>
+    <t>SENSOR DE POSICION DE ARBOL DE LEVAS</t>
+  </si>
+  <si>
+    <t>PASTILLAS DE FRENO</t>
+  </si>
+  <si>
+    <t>BUJIAS ATOS, I10, PICANTO 1RA C/U</t>
+  </si>
+  <si>
+    <t>VALVULAS DE ADMISION Y DE ESCAPE ATOS, I10, PICANTO 1RA C/U</t>
+  </si>
+  <si>
+    <t>CORREA AGREGADOS ATOS 4pk878</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TANQUE AUXILIAR DE RADIADOR ATOS </t>
+  </si>
+  <si>
+    <t>TAPA DE TANQUE AUXILIAR DE RADIADOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CABLE DE EMBRAGUE </t>
+  </si>
+  <si>
+    <t>BOTAS DE CREMALLERA PAREJA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CABLE DE EMERGENCIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TERMOSTATO </t>
+  </si>
+  <si>
+    <t>PARRILLAS DELANTERAS PICANTO 2DA PAREJA</t>
+  </si>
+  <si>
+    <t>SENSOR DE POSICION DE ARBOL DE LEVAS PICANTO 1RA</t>
+  </si>
+  <si>
+    <t>BUJIAS PICANTO 1RA, ATOS, I10 C/U</t>
+  </si>
+  <si>
+    <t>VALVULAS DE ADMISION Y DE ESCAPE PICANTO 1RA, ATOS, I10 C/U</t>
+  </si>
+  <si>
+    <t>MANGUERA DE RADIADOR SUPERIOR PICANTO 1RA(08-11)</t>
+  </si>
+  <si>
+    <t>MANGUERA DE RADIADOR INFERIOR PICANTO 1RA(08-11)</t>
+  </si>
+  <si>
+    <t>MANGUERA DE FRENO PICANTO 1RA</t>
+  </si>
+  <si>
+    <t>MANGUERA DE FRENO DELANTERA PICANTO 2DA</t>
+  </si>
+  <si>
+    <t>MANGUERA DE FRENO TRASERA PICANTO 2DA</t>
+  </si>
+  <si>
+    <t>CABLE DE EMERGENCIA PICANTO 1RA</t>
+  </si>
+  <si>
+    <t>CABLE DE EMERGENCIA PICANTO 2DA</t>
+  </si>
+  <si>
+    <t>FILTRO DE AIRE ACONDICIONADO PICANTO 1RA</t>
+  </si>
+  <si>
+    <t>TAMBORA PICANTO 2DA</t>
+  </si>
+  <si>
+    <t>ACEITE MOTOR SINTÉTICO 10W40 5L</t>
+  </si>
+  <si>
+    <t>ACEITE DE CAJA AUTOMÁTICA DEXRON III 5L</t>
   </si>
 </sst>
 </file>
@@ -1585,7 +1663,7 @@
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1630,6 +1708,10 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -1711,6 +1793,9 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1748,13 +1833,16 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1763,13 +1851,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -2048,13 +2130,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B276"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="88.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2075,7 +2158,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B3" s="2">
         <v>12</v>
@@ -2291,7 +2374,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B30" s="2">
         <v>80</v>
@@ -2315,7 +2398,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B33" s="2">
         <v>50</v>
@@ -2323,7 +2406,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B34" s="2">
         <v>12</v>
@@ -2379,7 +2462,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B41" s="2">
         <v>1</v>
@@ -2387,7 +2470,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B42" s="2">
         <v>1</v>
@@ -2395,7 +2478,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B43" s="2">
         <v>1</v>
@@ -2403,7 +2486,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B44" s="2">
         <v>10</v>
@@ -2435,7 +2518,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B48" s="2">
         <v>10</v>
@@ -2443,7 +2526,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B49" s="2">
         <v>10</v>
@@ -2651,7 +2734,7 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B75" s="2">
         <v>15</v>
@@ -2659,7 +2742,7 @@
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B76" s="2">
         <v>30</v>
@@ -2723,7 +2806,7 @@
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B84" s="2">
         <v>70</v>
@@ -2755,7 +2838,7 @@
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B88" s="2">
         <v>25</v>
@@ -2819,7 +2902,7 @@
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B96" s="2">
         <v>10</v>
@@ -2875,7 +2958,7 @@
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>283</v>
+        <v>499</v>
       </c>
       <c r="B103" s="2">
         <v>100</v>
@@ -2883,7 +2966,7 @@
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B104" s="2">
         <v>25</v>
@@ -2891,7 +2974,7 @@
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B105" s="2">
         <v>450</v>
@@ -2899,7 +2982,7 @@
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B106" s="2">
         <v>180</v>
@@ -2907,7 +2990,7 @@
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B107" s="2">
         <v>10</v>
@@ -2915,7 +2998,7 @@
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B108" s="2">
         <v>30</v>
@@ -2923,7 +3006,7 @@
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B109" s="2">
         <v>30</v>
@@ -2931,7 +3014,7 @@
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B110" s="2">
         <v>60</v>
@@ -2939,7 +3022,7 @@
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B111" s="2">
         <v>120</v>
@@ -2947,7 +3030,7 @@
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B112" s="2">
         <v>25</v>
@@ -2955,7 +3038,7 @@
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B113" s="2">
         <v>80</v>
@@ -2963,7 +3046,7 @@
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B114" s="2">
         <v>250</v>
@@ -2979,7 +3062,7 @@
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B116" s="2">
         <v>20</v>
@@ -2987,7 +3070,7 @@
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B117" s="2">
         <v>15</v>
@@ -2995,7 +3078,7 @@
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B118" s="2">
         <v>50</v>
@@ -3003,7 +3086,7 @@
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B119" s="2">
         <v>60</v>
@@ -3011,7 +3094,7 @@
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B120" s="2">
         <v>100</v>
@@ -3019,7 +3102,7 @@
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B121" s="2">
         <v>15</v>
@@ -3027,7 +3110,7 @@
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B122" s="2">
         <v>50</v>
@@ -3035,7 +3118,7 @@
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B123" s="2">
         <v>70</v>
@@ -3043,7 +3126,7 @@
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B124" s="2">
         <v>10</v>
@@ -3051,7 +3134,7 @@
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B125" s="2">
         <v>10</v>
@@ -3059,7 +3142,7 @@
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B126" s="2">
         <v>10</v>
@@ -3067,7 +3150,7 @@
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B127" s="2">
         <v>30</v>
@@ -3075,7 +3158,7 @@
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B128" s="2">
         <v>90</v>
@@ -3083,7 +3166,7 @@
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B129" s="2">
         <v>50</v>
@@ -3091,7 +3174,7 @@
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B130" s="2">
         <v>10</v>
@@ -3099,7 +3182,7 @@
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B131" s="2">
         <v>30</v>
@@ -3107,7 +3190,7 @@
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B132" s="2">
         <v>120</v>
@@ -3115,7 +3198,7 @@
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B133" s="2">
         <v>15</v>
@@ -3123,7 +3206,7 @@
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B134" s="2">
         <v>70</v>
@@ -3131,7 +3214,7 @@
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B135" s="2">
         <v>20</v>
@@ -3139,7 +3222,7 @@
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B136" s="2">
         <v>5</v>
@@ -3147,7 +3230,7 @@
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B137" s="2">
         <v>100</v>
@@ -3155,7 +3238,7 @@
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B138" s="2">
         <v>60</v>
@@ -3163,7 +3246,7 @@
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B139" s="2">
         <v>30</v>
@@ -3171,7 +3254,7 @@
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B140" s="2">
         <v>100</v>
@@ -3179,7 +3262,7 @@
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B141" s="2">
         <v>30</v>
@@ -3187,7 +3270,7 @@
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B142" s="2">
         <v>10</v>
@@ -3195,7 +3278,7 @@
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B143" s="2">
         <v>15</v>
@@ -3203,7 +3286,7 @@
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B144" s="2">
         <v>30</v>
@@ -3211,7 +3294,7 @@
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B145" s="2">
         <v>10</v>
@@ -3219,7 +3302,7 @@
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B146" s="2">
         <v>10</v>
@@ -3227,7 +3310,7 @@
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B147" s="2">
         <v>10</v>
@@ -3235,7 +3318,7 @@
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B148" s="2">
         <v>20</v>
@@ -3243,7 +3326,7 @@
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B149" s="2">
         <v>2</v>
@@ -3251,7 +3334,7 @@
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B150" s="2">
         <v>20</v>
@@ -3259,7 +3342,7 @@
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B151" s="2">
         <v>50</v>
@@ -3267,7 +3350,7 @@
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B152" s="2">
         <v>40</v>
@@ -3275,7 +3358,7 @@
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B153" s="2">
         <v>90</v>
@@ -3283,7 +3366,7 @@
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B154" s="2">
         <v>12</v>
@@ -3291,7 +3374,7 @@
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B155" s="2">
         <v>15</v>
@@ -3299,7 +3382,7 @@
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B156" s="2">
         <v>550</v>
@@ -3307,7 +3390,7 @@
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B157" s="2">
         <v>6</v>
@@ -3315,7 +3398,7 @@
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B158" s="2">
         <v>10</v>
@@ -3323,7 +3406,7 @@
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B159" s="2">
         <v>20</v>
@@ -3331,7 +3414,7 @@
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B160" s="2">
         <v>15</v>
@@ -3339,7 +3422,7 @@
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B161" s="2">
         <v>5</v>
@@ -3347,7 +3430,7 @@
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B162" s="2">
         <v>15</v>
@@ -3355,7 +3438,7 @@
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B163" s="2">
         <v>70</v>
@@ -3363,7 +3446,7 @@
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B164" s="2">
         <v>10</v>
@@ -3371,7 +3454,7 @@
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B165" s="2">
         <v>10</v>
@@ -3379,7 +3462,7 @@
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B166" s="2">
         <v>20</v>
@@ -3387,7 +3470,7 @@
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B167" s="2">
         <v>10</v>
@@ -3395,7 +3478,7 @@
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B168" s="2">
         <v>10</v>
@@ -3403,7 +3486,7 @@
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B169" s="2">
         <v>10</v>
@@ -3411,7 +3494,7 @@
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B170" s="2">
         <v>50</v>
@@ -3419,7 +3502,7 @@
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B171" s="2">
         <v>30</v>
@@ -3427,7 +3510,7 @@
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B172" s="2">
         <v>7</v>
@@ -3435,7 +3518,7 @@
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B173" s="2">
         <v>280</v>
@@ -3443,7 +3526,7 @@
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B174" s="2">
         <v>150</v>
@@ -3451,7 +3534,7 @@
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B175" s="2">
         <v>80</v>
@@ -3459,7 +3542,7 @@
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B176" s="2">
         <v>30</v>
@@ -3467,7 +3550,7 @@
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B177" s="2">
         <v>150</v>
@@ -3475,7 +3558,7 @@
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B178" s="2">
         <v>10</v>
@@ -3483,7 +3566,7 @@
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B179" s="2">
         <v>10</v>
@@ -3491,7 +3574,7 @@
     </row>
     <row r="180" spans="1:2">
       <c r="A180" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B180" s="2">
         <v>20</v>
@@ -3499,7 +3582,7 @@
     </row>
     <row r="181" spans="1:2">
       <c r="A181" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B181" s="2">
         <v>100</v>
@@ -3507,7 +3590,7 @@
     </row>
     <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B182" s="2">
         <v>120</v>
@@ -3515,7 +3598,7 @@
     </row>
     <row r="183" spans="1:2">
       <c r="A183" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B183" s="2">
         <v>300</v>
@@ -3523,7 +3606,7 @@
     </row>
     <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B184" s="2">
         <v>160</v>
@@ -3531,7 +3614,7 @@
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B185" s="2">
         <v>110</v>
@@ -3539,7 +3622,7 @@
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B186" s="2">
         <v>160</v>
@@ -3547,7 +3630,7 @@
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B187" s="2">
         <v>30</v>
@@ -3555,7 +3638,7 @@
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B188" s="2">
         <v>170</v>
@@ -3563,7 +3646,7 @@
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B189" s="2">
         <v>80</v>
@@ -3571,7 +3654,7 @@
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B190" s="2">
         <v>220</v>
@@ -3579,7 +3662,7 @@
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B191" s="2">
         <v>90</v>
@@ -3587,7 +3670,7 @@
     </row>
     <row r="192" spans="1:2">
       <c r="A192" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B192" s="2">
         <v>25</v>
@@ -3595,7 +3678,7 @@
     </row>
     <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B193" s="2">
         <v>70</v>
@@ -3603,7 +3686,7 @@
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B194" s="2">
         <v>25</v>
@@ -3611,7 +3694,7 @@
     </row>
     <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B195" s="2">
         <v>10</v>
@@ -3619,7 +3702,7 @@
     </row>
     <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B196" s="2">
         <v>30</v>
@@ -3627,7 +3710,7 @@
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B197" s="2">
         <v>30</v>
@@ -3635,7 +3718,7 @@
     </row>
     <row r="198" spans="1:2">
       <c r="A198" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B198" s="2">
         <v>60</v>
@@ -3643,7 +3726,7 @@
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B199" s="2">
         <v>40</v>
@@ -3651,7 +3734,7 @@
     </row>
     <row r="200" spans="1:2">
       <c r="A200" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B200" s="2">
         <v>30</v>
@@ -3659,7 +3742,7 @@
     </row>
     <row r="201" spans="1:2">
       <c r="A201" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B201" s="2">
         <v>20</v>
@@ -3667,7 +3750,7 @@
     </row>
     <row r="202" spans="1:2">
       <c r="A202" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B202" s="2">
         <v>20</v>
@@ -3675,7 +3758,7 @@
     </row>
     <row r="203" spans="1:2">
       <c r="A203" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B203" s="2">
         <v>150</v>
@@ -3683,7 +3766,7 @@
     </row>
     <row r="204" spans="1:2">
       <c r="A204" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B204" s="2">
         <v>350</v>
@@ -3691,7 +3774,7 @@
     </row>
     <row r="205" spans="1:2">
       <c r="A205" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B205" s="2">
         <v>20</v>
@@ -3699,7 +3782,7 @@
     </row>
     <row r="206" spans="1:2">
       <c r="A206" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B206" s="2">
         <v>20</v>
@@ -3707,7 +3790,7 @@
     </row>
     <row r="207" spans="1:2">
       <c r="A207" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B207" s="2">
         <v>15</v>
@@ -3715,7 +3798,7 @@
     </row>
     <row r="208" spans="1:2">
       <c r="A208" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B208" s="2">
         <v>30</v>
@@ -3723,7 +3806,7 @@
     </row>
     <row r="209" spans="1:2">
       <c r="A209" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B209" s="2">
         <v>15</v>
@@ -3731,7 +3814,7 @@
     </row>
     <row r="210" spans="1:2">
       <c r="A210" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B210" s="2">
         <v>70</v>
@@ -3739,7 +3822,7 @@
     </row>
     <row r="211" spans="1:2">
       <c r="A211" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B211" s="2">
         <v>40</v>
@@ -3747,7 +3830,7 @@
     </row>
     <row r="212" spans="1:2">
       <c r="A212" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B212" s="2">
         <v>100</v>
@@ -3755,7 +3838,7 @@
     </row>
     <row r="213" spans="1:2">
       <c r="A213" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B213" s="2">
         <v>70</v>
@@ -3763,7 +3846,7 @@
     </row>
     <row r="214" spans="1:2">
       <c r="A214" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B214" s="2">
         <v>15</v>
@@ -3771,7 +3854,7 @@
     </row>
     <row r="215" spans="1:2">
       <c r="A215" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B215" s="2">
         <v>130</v>
@@ -3779,7 +3862,7 @@
     </row>
     <row r="216" spans="1:2">
       <c r="A216" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B216" s="2">
         <v>200</v>
@@ -3787,7 +3870,7 @@
     </row>
     <row r="217" spans="1:2">
       <c r="A217" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B217" s="2">
         <v>30</v>
@@ -3795,7 +3878,7 @@
     </row>
     <row r="218" spans="1:2">
       <c r="A218" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B218" s="2">
         <v>15</v>
@@ -3803,7 +3886,7 @@
     </row>
     <row r="219" spans="1:2">
       <c r="A219" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B219" s="2">
         <v>65</v>
@@ -3811,7 +3894,7 @@
     </row>
     <row r="220" spans="1:2">
       <c r="A220" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B220" s="2">
         <v>95</v>
@@ -3819,7 +3902,7 @@
     </row>
     <row r="221" spans="1:2">
       <c r="A221" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B221" s="2">
         <v>10</v>
@@ -3827,7 +3910,7 @@
     </row>
     <row r="222" spans="1:2">
       <c r="A222" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B222" s="2">
         <v>20</v>
@@ -3835,7 +3918,7 @@
     </row>
     <row r="223" spans="1:2">
       <c r="A223" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B223" s="2">
         <v>10</v>
@@ -3843,7 +3926,7 @@
     </row>
     <row r="224" spans="1:2">
       <c r="A224" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B224" s="2">
         <v>10</v>
@@ -3851,7 +3934,7 @@
     </row>
     <row r="225" spans="1:2">
       <c r="A225" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B225" s="2">
         <v>10</v>
@@ -3859,7 +3942,7 @@
     </row>
     <row r="226" spans="1:2">
       <c r="A226" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B226" s="2">
         <v>10</v>
@@ -3867,7 +3950,7 @@
     </row>
     <row r="227" spans="1:2">
       <c r="A227" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B227" s="2">
         <v>15</v>
@@ -3875,7 +3958,7 @@
     </row>
     <row r="228" spans="1:2">
       <c r="A228" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B228" s="2">
         <v>15</v>
@@ -3883,7 +3966,7 @@
     </row>
     <row r="229" spans="1:2">
       <c r="A229" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B229" s="2">
         <v>15</v>
@@ -3891,7 +3974,7 @@
     </row>
     <row r="230" spans="1:2">
       <c r="A230" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B230" s="2">
         <v>15</v>
@@ -3899,7 +3982,7 @@
     </row>
     <row r="231" spans="1:2">
       <c r="A231" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B231" s="2">
         <v>6</v>
@@ -3907,7 +3990,7 @@
     </row>
     <row r="232" spans="1:2">
       <c r="A232" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B232" s="2">
         <v>10</v>
@@ -3915,7 +3998,7 @@
     </row>
     <row r="233" spans="1:2">
       <c r="A233" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B233" s="2">
         <v>150</v>
@@ -3923,7 +4006,7 @@
     </row>
     <row r="234" spans="1:2">
       <c r="A234" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B234" s="2">
         <v>180</v>
@@ -3931,7 +4014,7 @@
     </row>
     <row r="235" spans="1:2">
       <c r="A235" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B235" s="2">
         <v>90</v>
@@ -3939,7 +4022,7 @@
     </row>
     <row r="236" spans="1:2">
       <c r="A236" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B236" s="2">
         <v>30</v>
@@ -3947,7 +4030,7 @@
     </row>
     <row r="237" spans="1:2">
       <c r="A237" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B237" s="2">
         <v>25</v>
@@ -3955,7 +4038,7 @@
     </row>
     <row r="238" spans="1:2">
       <c r="A238" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B238" s="2">
         <v>4</v>
@@ -3963,7 +4046,7 @@
     </row>
     <row r="239" spans="1:2">
       <c r="A239" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B239" s="2">
         <v>75</v>
@@ -3971,7 +4054,7 @@
     </row>
     <row r="240" spans="1:2">
       <c r="A240" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B240" s="2">
         <v>25</v>
@@ -3979,7 +4062,7 @@
     </row>
     <row r="241" spans="1:2">
       <c r="A241" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B241" s="2">
         <v>70</v>
@@ -3987,7 +4070,7 @@
     </row>
     <row r="242" spans="1:2">
       <c r="A242" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B242" s="2">
         <v>15</v>
@@ -3995,7 +4078,7 @@
     </row>
     <row r="243" spans="1:2">
       <c r="A243" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B243" s="2">
         <v>250</v>
@@ -4003,7 +4086,7 @@
     </row>
     <row r="244" spans="1:2">
       <c r="A244" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B244" s="2">
         <v>550</v>
@@ -4011,7 +4094,7 @@
     </row>
     <row r="245" spans="1:2">
       <c r="A245" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B245" s="2">
         <v>25</v>
@@ -4019,7 +4102,7 @@
     </row>
     <row r="246" spans="1:2">
       <c r="A246" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B246" s="2">
         <v>10</v>
@@ -4027,7 +4110,7 @@
     </row>
     <row r="247" spans="1:2">
       <c r="A247" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B247" s="2">
         <v>10</v>
@@ -4035,7 +4118,7 @@
     </row>
     <row r="248" spans="1:2">
       <c r="A248" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B248" s="2">
         <v>15</v>
@@ -4043,7 +4126,7 @@
     </row>
     <row r="249" spans="1:2">
       <c r="A249" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B249" s="2">
         <v>7</v>
@@ -4051,7 +4134,7 @@
     </row>
     <row r="250" spans="1:2">
       <c r="A250" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B250" s="2">
         <v>50</v>
@@ -4059,7 +4142,7 @@
     </row>
     <row r="251" spans="1:2">
       <c r="A251" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B251" s="2">
         <v>5</v>
@@ -4067,7 +4150,7 @@
     </row>
     <row r="252" spans="1:2">
       <c r="A252" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B252" s="2">
         <v>5</v>
@@ -4075,7 +4158,7 @@
     </row>
     <row r="253" spans="1:2">
       <c r="A253" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B253" s="2">
         <v>5</v>
@@ -4083,7 +4166,7 @@
     </row>
     <row r="254" spans="1:2">
       <c r="A254" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B254" s="2">
         <v>7</v>
@@ -4091,7 +4174,7 @@
     </row>
     <row r="255" spans="1:2">
       <c r="A255" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B255" s="2">
         <v>20</v>
@@ -4099,7 +4182,7 @@
     </row>
     <row r="256" spans="1:2">
       <c r="A256" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B256" s="2">
         <v>10</v>
@@ -4107,7 +4190,7 @@
     </row>
     <row r="257" spans="1:2">
       <c r="A257" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B257" s="2">
         <v>15</v>
@@ -4115,7 +4198,7 @@
     </row>
     <row r="258" spans="1:2">
       <c r="A258" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B258" s="2">
         <v>5</v>
@@ -4123,7 +4206,7 @@
     </row>
     <row r="259" spans="1:2">
       <c r="A259" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B259" s="2">
         <v>7</v>
@@ -4131,7 +4214,7 @@
     </row>
     <row r="260" spans="1:2">
       <c r="A260" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B260" s="2">
         <v>10</v>
@@ -4139,7 +4222,7 @@
     </row>
     <row r="261" spans="1:2">
       <c r="A261" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B261" s="2">
         <v>2</v>
@@ -4147,7 +4230,7 @@
     </row>
     <row r="262" spans="1:2">
       <c r="A262" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B262" s="2">
         <v>5</v>
@@ -4155,7 +4238,7 @@
     </row>
     <row r="263" spans="1:2">
       <c r="A263" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B263" s="2">
         <v>3</v>
@@ -4163,7 +4246,7 @@
     </row>
     <row r="264" spans="1:2">
       <c r="A264" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B264" s="2">
         <v>4</v>
@@ -4171,7 +4254,7 @@
     </row>
     <row r="265" spans="1:2">
       <c r="A265" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B265" s="2">
         <v>3</v>
@@ -4179,7 +4262,7 @@
     </row>
     <row r="266" spans="1:2">
       <c r="A266" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B266" s="2">
         <v>2</v>
@@ -4187,7 +4270,7 @@
     </row>
     <row r="267" spans="1:2">
       <c r="A267" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B267" s="2">
         <v>20</v>
@@ -4195,7 +4278,7 @@
     </row>
     <row r="268" spans="1:2">
       <c r="A268" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B268" s="2">
         <v>25</v>
@@ -4203,7 +4286,7 @@
     </row>
     <row r="269" spans="1:2">
       <c r="A269" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B269" s="2">
         <v>45</v>
@@ -4211,7 +4294,7 @@
     </row>
     <row r="270" spans="1:2">
       <c r="A270" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B270" s="2">
         <v>15</v>
@@ -4219,7 +4302,7 @@
     </row>
     <row r="271" spans="1:2">
       <c r="A271" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B271" s="2">
         <v>60</v>
@@ -4227,7 +4310,7 @@
     </row>
     <row r="272" spans="1:2">
       <c r="A272" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B272" s="2">
         <v>100</v>
@@ -4235,7 +4318,7 @@
     </row>
     <row r="273" spans="1:2">
       <c r="A273" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B273" s="2">
         <v>35</v>
@@ -4243,7 +4326,7 @@
     </row>
     <row r="274" spans="1:2">
       <c r="A274" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B274" s="2">
         <v>10</v>
@@ -4251,7 +4334,7 @@
     </row>
     <row r="275" spans="1:2">
       <c r="A275" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B275" s="2">
         <v>10</v>
@@ -4259,26 +4342,23 @@
     </row>
     <row r="276" spans="1:2">
       <c r="A276" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B276" s="2">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:B276">
-    <sortCondition ref="A3:A276"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15"/>
@@ -4353,7 +4433,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="7" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B9" s="5">
         <v>80</v>
@@ -4393,7 +4473,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="7" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B14" s="5">
         <v>1</v>
@@ -4401,7 +4481,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B15" s="5">
         <v>1</v>
@@ -4409,7 +4489,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
@@ -4417,183 +4497,183 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="7" t="s">
-        <v>13</v>
+        <v>508</v>
       </c>
       <c r="B17" s="5">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="7" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B18" s="5">
-        <v>2.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="7" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B19" s="5">
-        <v>10</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="B21" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B22" s="5">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="5">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="5">
-        <v>35</v>
-      </c>
-    </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="10" t="s">
-        <v>47</v>
+      <c r="A23" s="7" t="s">
+        <v>507</v>
       </c>
       <c r="B23" s="5">
-        <v>140</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="8" t="s">
-        <v>149</v>
+      <c r="A24" s="7" t="s">
+        <v>509</v>
       </c>
       <c r="B24" s="5">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="5">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="B28" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B29" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B30" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>495</v>
-      </c>
-      <c r="B26" s="31">
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>494</v>
+      </c>
+      <c r="B31" s="12">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="6" t="s">
+    <row r="32" spans="1:2">
+      <c r="A32" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B32" s="5">
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="12" t="s">
+    <row r="33" spans="1:2">
+      <c r="A33" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B33" s="5">
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="6" t="s">
+    <row r="34" spans="1:2">
+      <c r="A34" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B34" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="11" t="s">
+    <row r="35" spans="1:2">
+      <c r="A35" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B35" s="5">
         <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" s="5">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>494</v>
-      </c>
-      <c r="B32" s="31">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B33" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B35" s="5">
-        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="14" t="s">
-        <v>157</v>
+        <v>16</v>
       </c>
       <c r="B36" s="5">
-        <v>15</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="B37" s="5">
-        <v>80</v>
+      <c r="A37" t="s">
+        <v>493</v>
+      </c>
+      <c r="B37" s="12">
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="7" t="s">
-        <v>4</v>
+      <c r="A38" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="B38" s="5">
-        <v>120</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="9" t="s">
-        <v>19</v>
+      <c r="A39" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="B39" s="5">
         <v>10</v>
@@ -4601,175 +4681,263 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B41" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B42" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B45" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B41" s="5">
+    <row r="46" spans="1:2">
+      <c r="A46" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="9" t="s">
+    <row r="47" spans="1:2">
+      <c r="A47" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B47" s="5">
         <v>25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B43" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B44" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="B45" s="5">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="B46" s="5">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" s="5">
-        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B50" s="5">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B51" s="5">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="5">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B53" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="11" t="s">
+    <row r="54" spans="1:2">
+      <c r="A54" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="B54" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B55" s="5">
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="9" t="s">
+    <row r="56" spans="1:2">
+      <c r="A56" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B50" s="5">
+      <c r="B56" s="5">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
-        <v>493</v>
-      </c>
-      <c r="B51" s="31">
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>492</v>
+      </c>
+      <c r="B57" s="12">
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="10" t="s">
+    <row r="58" spans="1:2">
+      <c r="A58" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B58" s="5">
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="15" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B59" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="15" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B60" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="15" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="B55" s="5">
+      <c r="B61" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="18" t="s">
+    <row r="62" spans="1:2">
+      <c r="A62" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="B56" s="5">
+      <c r="B62" s="5">
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="9" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="B63" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="B64" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B57" s="5">
+      <c r="B65" s="5">
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="19" t="s">
+    <row r="66" spans="1:2">
+      <c r="A66" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="B66" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B67" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" t="s">
-        <v>466</v>
-      </c>
-      <c r="B59" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="7" t="s">
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>465</v>
+      </c>
+      <c r="B68" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="B69" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="B70" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B60" s="5">
+      <c r="B71" s="5">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B60">
-    <sortCondition ref="A2:A60"/>
+  <sortState ref="A3:B71">
+    <sortCondition ref="A3:A71"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4777,10 +4945,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B156"/>
+  <dimension ref="A1:B169"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15"/>
@@ -4790,15 +4958,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="5">
@@ -4806,7 +4974,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="5">
@@ -4814,7 +4982,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>145</v>
       </c>
       <c r="B4" s="5">
@@ -4822,7 +4990,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="16" t="s">
         <v>158</v>
       </c>
       <c r="B5" s="5">
@@ -4830,7 +4998,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="5">
@@ -4838,7 +5006,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="22" t="s">
         <v>188</v>
       </c>
       <c r="B7" s="5">
@@ -4846,7 +5014,7 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="16" t="s">
         <v>102</v>
       </c>
       <c r="B8" s="5">
@@ -4854,7 +5022,7 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="24" t="s">
         <v>197</v>
       </c>
       <c r="B9" s="5">
@@ -4862,7 +5030,7 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="16" t="s">
         <v>159</v>
       </c>
       <c r="B10" s="5">
@@ -4870,7 +5038,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="16" t="s">
         <v>160</v>
       </c>
       <c r="B11" s="5">
@@ -4878,7 +5046,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="5">
@@ -4886,15 +5054,15 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="15" t="s">
-        <v>499</v>
+      <c r="A13" s="16" t="s">
+        <v>498</v>
       </c>
       <c r="B13" s="5">
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="16" t="s">
         <v>194</v>
       </c>
       <c r="B14" s="5">
@@ -4902,7 +5070,7 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="16" t="s">
         <v>103</v>
       </c>
       <c r="B15" s="5">
@@ -4910,23 +5078,23 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="16" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="5">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="5">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="24" t="s">
         <v>144</v>
       </c>
       <c r="B18" s="5">
@@ -4934,7 +5102,7 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="16" t="s">
         <v>161</v>
       </c>
       <c r="B19" s="5">
@@ -4942,7 +5110,7 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B20" s="5">
@@ -4950,7 +5118,7 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B21" s="5">
@@ -4958,7 +5126,7 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="16" t="s">
         <v>44</v>
       </c>
       <c r="B22" s="5">
@@ -4966,7 +5134,7 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="16" t="s">
         <v>189</v>
       </c>
       <c r="B23" s="5">
@@ -4974,7 +5142,7 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="23" t="s">
         <v>38</v>
       </c>
       <c r="B24" s="5">
@@ -4982,16 +5150,16 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="15" t="s">
-        <v>470</v>
+      <c r="A25" s="16" t="s">
+        <v>469</v>
       </c>
       <c r="B25" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="15" t="s">
-        <v>471</v>
+      <c r="A26" s="16" t="s">
+        <v>470</v>
       </c>
       <c r="B26" s="5">
         <v>1</v>
@@ -4999,14 +5167,14 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="16" t="s">
         <v>105</v>
       </c>
       <c r="B28" s="5">
@@ -5014,7 +5182,7 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="16" t="s">
         <v>104</v>
       </c>
       <c r="B29" s="5">
@@ -5022,7 +5190,7 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="16" t="s">
         <v>106</v>
       </c>
       <c r="B30" s="5">
@@ -5030,7 +5198,7 @@
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="16" t="s">
         <v>162</v>
       </c>
       <c r="B31" s="5">
@@ -5038,7 +5206,7 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="16" t="s">
         <v>163</v>
       </c>
       <c r="B32" s="5">
@@ -5046,7 +5214,7 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="16" t="s">
         <v>107</v>
       </c>
       <c r="B33" s="5">
@@ -5054,992 +5222,1096 @@
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="16" t="s">
+        <v>513</v>
+      </c>
+      <c r="B34" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="25" t="s">
         <v>164</v>
-      </c>
-      <c r="B34" s="5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="22" t="s">
-        <v>165</v>
       </c>
       <c r="B35" s="5">
         <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="16" t="s">
+        <v>520</v>
+      </c>
+      <c r="B36" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="16" t="s">
+        <v>521</v>
+      </c>
+      <c r="B37" s="5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="B38" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B39" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="15" t="s">
+    <row r="40" spans="1:2">
+      <c r="A40" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B40" s="5">
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="15" t="s">
+    <row r="41" spans="1:2">
+      <c r="A41" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B41" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="21" t="s">
+    <row r="42" spans="1:2">
+      <c r="A42" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B42" s="5">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="15" t="s">
+    <row r="43" spans="1:2">
+      <c r="A43" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B43" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="15" t="s">
+    <row r="44" spans="1:2">
+      <c r="A44" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B44" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="24" t="s">
+    <row r="45" spans="1:2">
+      <c r="A45" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B45" s="5">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="15" t="s">
+    <row r="46" spans="1:2">
+      <c r="A46" s="16" t="s">
         <v>50</v>
-      </c>
-      <c r="B43" s="5">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="5">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="5">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="15" t="s">
-        <v>51</v>
       </c>
       <c r="B46" s="5">
         <v>160</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="23" t="s">
+      <c r="A47" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="5">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="5">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="5">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B50" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="15" t="s">
+    <row r="51" spans="1:2">
+      <c r="A51" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B51" s="5">
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="15" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B52" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="15" t="s">
+    <row r="53" spans="1:2">
+      <c r="A53" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="5">
+      <c r="B53" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="15" t="s">
+    <row r="54" spans="1:2">
+      <c r="A54" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B54" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="15" t="s">
+    <row r="55" spans="1:2">
+      <c r="A55" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B55" s="5">
         <v>150</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="15" t="s">
+    <row r="56" spans="1:2">
+      <c r="A56" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B56" s="5">
         <v>200</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="15" t="s">
+    <row r="57" spans="1:2">
+      <c r="A57" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B57" s="5">
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="15" t="s">
+    <row r="58" spans="1:2">
+      <c r="A58" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="5">
+      <c r="B58" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="15" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B56" s="5">
+      <c r="B59" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="15" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B57" s="5">
+      <c r="B60" s="5">
         <v>160</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="15" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B61" s="5">
         <v>160</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="15" t="s">
+    <row r="62" spans="1:2">
+      <c r="A62" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="B59" s="5">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B60" s="5">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B61" s="5">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="15" t="s">
-        <v>61</v>
       </c>
       <c r="B62" s="5">
         <v>250</v>
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="15" t="s">
-        <v>62</v>
+      <c r="A63" s="16" t="s">
+        <v>59</v>
       </c>
       <c r="B63" s="5">
         <v>250</v>
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="15" t="s">
+      <c r="A64" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B64" s="5">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B65" s="5">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B66" s="5">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B64" s="5">
+      <c r="B67" s="5">
         <v>250</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="15" t="s">
+    <row r="68" spans="1:2">
+      <c r="A68" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B65" s="5">
+      <c r="B68" s="5">
         <v>150</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="15" t="s">
+    <row r="69" spans="1:2">
+      <c r="A69" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="5">
+      <c r="B69" s="5">
         <v>200</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="15" t="s">
+    <row r="70" spans="1:2">
+      <c r="A70" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="5">
+      <c r="B70" s="5">
         <v>220</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="15" t="s">
+    <row r="71" spans="1:2">
+      <c r="A71" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="5">
+      <c r="B71" s="5">
         <v>220</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="15" t="s">
+    <row r="72" spans="1:2">
+      <c r="A72" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="5">
+      <c r="B72" s="5">
         <v>220</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="15" t="s">
+    <row r="73" spans="1:2">
+      <c r="A73" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B70" s="5">
+      <c r="B73" s="5">
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="24" t="s">
+    <row r="74" spans="1:2">
+      <c r="A74" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="B71" s="5">
+      <c r="B74" s="5">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="15" t="s">
+    <row r="75" spans="1:2">
+      <c r="A75" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B72" s="5">
+      <c r="B75" s="5">
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="15" t="s">
+    <row r="76" spans="1:2">
+      <c r="A76" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B73" s="5">
+      <c r="B76" s="5">
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="15" t="s">
+    <row r="77" spans="1:2">
+      <c r="A77" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B74" s="5">
+      <c r="B77" s="5">
         <v>180</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="32" t="s">
-        <v>497</v>
-      </c>
-      <c r="B75" s="31">
+    <row r="78" spans="1:2">
+      <c r="A78" s="26" t="s">
+        <v>496</v>
+      </c>
+      <c r="B78" s="12">
         <v>50</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="15" t="s">
+    <row r="79" spans="1:2">
+      <c r="A79" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="B76" s="5">
+      <c r="B79" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="15" t="s">
+    <row r="80" spans="1:2">
+      <c r="A80" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="B77" s="5">
+      <c r="B80" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="15" t="s">
+    <row r="81" spans="1:2">
+      <c r="A81" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="B78" s="5">
+      <c r="B81" s="5">
         <v>120</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="15" t="s">
+    <row r="82" spans="1:2">
+      <c r="A82" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="B79" s="5">
+      <c r="B82" s="5">
         <v>150</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
-      <c r="A80" s="22" t="s">
+    <row r="83" spans="1:2">
+      <c r="A83" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="B80" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="15" t="s">
+      <c r="B83" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="B81" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="15" t="s">
+      <c r="B84" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="16" t="s">
+        <v>522</v>
+      </c>
+      <c r="B85" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B82" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="15" t="s">
+      <c r="B86" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B83" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="15" t="s">
+      <c r="B87" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B84" s="5">
+      <c r="B88" s="5">
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="15" t="s">
+    <row r="89" spans="1:2">
+      <c r="A89" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="B85" s="5">
+      <c r="B89" s="5">
         <v>80</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="15" t="s">
-        <v>491</v>
-      </c>
-      <c r="B86" s="5">
+    <row r="90" spans="1:2">
+      <c r="A90" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="B90" s="5">
         <v>80</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="15" t="s">
+    <row r="91" spans="1:2">
+      <c r="A91" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B87" s="5">
+      <c r="B91" s="5">
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
-      <c r="A88" s="15" t="s">
+    <row r="92" spans="1:2">
+      <c r="A92" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B88" s="5">
+      <c r="B92" s="5">
         <v>25</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="25" t="s">
+    <row r="93" spans="1:2">
+      <c r="A93" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="B89" s="5">
+      <c r="B93" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="15" t="s">
+    <row r="94" spans="1:2">
+      <c r="A94" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B90" s="5">
+      <c r="B94" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="15" t="s">
+    <row r="95" spans="1:2">
+      <c r="A95" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B91" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="26" t="s">
+      <c r="B95" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B92" s="5">
+      <c r="B96" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="15" t="s">
+    <row r="97" spans="1:2">
+      <c r="A97" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="B93" s="5">
+      <c r="B97" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="B94" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="B95" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B96" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B97" s="5">
-        <v>15</v>
-      </c>
-    </row>
     <row r="98" spans="1:2">
-      <c r="A98" s="15" t="s">
-        <v>115</v>
+      <c r="A98" s="16" t="s">
+        <v>518</v>
       </c>
       <c r="B98" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="99" spans="1:2">
-      <c r="A99" s="15" t="s">
-        <v>117</v>
+      <c r="A99" s="16" t="s">
+        <v>517</v>
       </c>
       <c r="B99" s="5">
         <v>15</v>
       </c>
     </row>
     <row r="100" spans="1:2">
-      <c r="A100" s="15" t="s">
+      <c r="A100" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="B100" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="16" t="s">
+        <v>516</v>
+      </c>
+      <c r="B101" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B102" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="16" t="s">
+        <v>515</v>
+      </c>
+      <c r="B103" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="B104" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B105" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B106" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B107" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B108" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="B100" s="5">
+      <c r="B109" s="5">
         <v>250</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
-      <c r="A101" s="23" t="s">
+    <row r="110" spans="1:2">
+      <c r="A110" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="B101" s="5">
+      <c r="B110" s="5">
         <v>140</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
-      <c r="A102" s="15" t="s">
+    <row r="111" spans="1:2">
+      <c r="A111" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="B102" s="5">
+      <c r="B111" s="5">
         <v>150</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
-      <c r="A103" s="15" t="s">
+    <row r="112" spans="1:2">
+      <c r="A112" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B103" s="5">
+      <c r="B112" s="5">
         <v>150</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
-      <c r="A104" s="15" t="s">
+    <row r="113" spans="1:2">
+      <c r="A113" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="B104" s="5">
+      <c r="B113" s="5">
         <v>140</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
-      <c r="A105" s="15" t="s">
+    <row r="114" spans="1:2">
+      <c r="A114" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B105" s="5">
+      <c r="B114" s="5">
         <v>120</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
-      <c r="A106" s="15" t="s">
+    <row r="115" spans="1:2">
+      <c r="A115" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B106" s="5">
+      <c r="B115" s="5">
         <v>200</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
-      <c r="A107" s="15" t="s">
+    <row r="116" spans="1:2">
+      <c r="A116" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="B107" s="5">
+      <c r="B116" s="5">
         <v>230</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
-      <c r="A108" s="15" t="s">
+    <row r="117" spans="1:2">
+      <c r="A117" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B108" s="5">
+      <c r="B117" s="5">
         <v>350</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
-      <c r="A109" s="27" t="s">
+    <row r="118" spans="1:2">
+      <c r="A118" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="B109" s="5">
+      <c r="B118" s="5">
         <v>180</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
-      <c r="A110" s="15" t="s">
+    <row r="119" spans="1:2">
+      <c r="A119" s="16" t="s">
+        <v>511</v>
+      </c>
+      <c r="B119" s="5">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="B110" s="5">
+      <c r="B120" s="5">
         <v>35</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
-      <c r="A111" s="15" t="s">
+    <row r="121" spans="1:2">
+      <c r="A121" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="B111" s="5">
+      <c r="B121" s="5">
         <v>35</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
-      <c r="A112" s="15" t="s">
+    <row r="122" spans="1:2">
+      <c r="A122" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B112" s="5">
+      <c r="B122" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
-      <c r="A113" s="24" t="s">
+    <row r="123" spans="1:2">
+      <c r="A123" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="B113" s="5">
+      <c r="B123" s="5">
         <v>70</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
-      <c r="A114" s="28" t="s">
+    <row r="124" spans="1:2">
+      <c r="A124" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="B114" s="5">
+      <c r="B124" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
-      <c r="A115" s="15" t="s">
+    <row r="125" spans="1:2">
+      <c r="A125" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="B115" s="5">
+      <c r="B125" s="5">
         <v>45</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
-      <c r="A116" s="15" t="s">
+    <row r="126" spans="1:2">
+      <c r="A126" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="B116" s="5">
+      <c r="B126" s="5">
         <v>25</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
-      <c r="A117" s="15" t="s">
+    <row r="127" spans="1:2">
+      <c r="A127" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="B117" s="5">
+      <c r="B127" s="5">
         <v>45</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
-      <c r="A118" s="32" t="s">
-        <v>496</v>
-      </c>
-      <c r="B118" s="31">
+    <row r="128" spans="1:2">
+      <c r="A128" s="26" t="s">
+        <v>495</v>
+      </c>
+      <c r="B128" s="12">
         <v>150</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
-      <c r="A119" s="15" t="s">
+    <row r="129" spans="1:2">
+      <c r="A129" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B119" s="5">
+      <c r="B129" s="5">
         <v>160</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
-      <c r="A120" s="15" t="s">
+    <row r="130" spans="1:2">
+      <c r="A130" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="B120" s="5">
+      <c r="B130" s="5">
         <v>150</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
-      <c r="A121" s="15" t="s">
+    <row r="131" spans="1:2">
+      <c r="A131" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B121" s="5">
+      <c r="B131" s="5">
         <v>200</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
-      <c r="A122" s="15" t="s">
+    <row r="132" spans="1:2">
+      <c r="A132" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="B122" s="5">
+      <c r="B132" s="5">
         <v>140</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
-      <c r="A123" s="15" t="s">
+    <row r="133" spans="1:2">
+      <c r="A133" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B123" s="5">
+      <c r="B133" s="5">
         <v>130</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
-      <c r="A124" s="15" t="s">
+    <row r="134" spans="1:2">
+      <c r="A134" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B124" s="5">
+      <c r="B134" s="5">
         <v>80</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
-      <c r="A125" s="15" t="s">
+    <row r="135" spans="1:2">
+      <c r="A135" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B125" s="5">
+      <c r="B135" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
-      <c r="A126" s="15" t="s">
+    <row r="136" spans="1:2">
+      <c r="A136" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B126" s="5">
+      <c r="B136" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
-      <c r="A127" s="15" t="s">
+    <row r="137" spans="1:2">
+      <c r="A137" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B127" s="5">
+      <c r="B137" s="5">
         <v>120</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
-      <c r="A128" s="15" t="s">
+    <row r="138" spans="1:2">
+      <c r="A138" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B128" s="5">
+      <c r="B138" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
-      <c r="A129" s="15" t="s">
+    <row r="139" spans="1:2">
+      <c r="A139" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B129" s="5">
+      <c r="B139" s="5">
         <v>120</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
-      <c r="A130" s="15" t="s">
+    <row r="140" spans="1:2">
+      <c r="A140" s="16" t="s">
         <v>126</v>
-      </c>
-      <c r="B130" s="5">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2">
-      <c r="A131" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="B131" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2">
-      <c r="A132" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="B132" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2">
-      <c r="A133" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B133" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2">
-      <c r="A134" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="B134" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2">
-      <c r="A135" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="B135" s="5">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2">
-      <c r="A136" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="B136" s="5">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2">
-      <c r="A137" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="B137" s="5">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2">
-      <c r="A138" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="B138" s="5">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2">
-      <c r="A139" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="B139" s="5">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2">
-      <c r="A140" s="15" t="s">
-        <v>131</v>
       </c>
       <c r="B140" s="5">
         <v>180</v>
       </c>
     </row>
     <row r="141" spans="1:2">
-      <c r="A141" s="15" t="s">
+      <c r="A141" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B141" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="B142" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B143" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="B144" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B145" s="5">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B146" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B147" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="B148" s="5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B149" s="5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B150" s="5">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B141" s="5">
+      <c r="B151" s="5">
         <v>180</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
-      <c r="A142" s="25" t="s">
+    <row r="152" spans="1:2">
+      <c r="A152" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="B142" s="5">
+      <c r="B152" s="5">
         <v>35</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
-      <c r="A143" s="15" t="s">
+    <row r="153" spans="1:2">
+      <c r="A153" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="B143" s="5">
+      <c r="B153" s="5">
         <v>35</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
-      <c r="A144" s="15" t="s">
+    <row r="154" spans="1:2">
+      <c r="A154" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B144" s="5">
+      <c r="B154" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
-      <c r="A145" s="15" t="s">
+    <row r="155" spans="1:2">
+      <c r="A155" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B145" s="5">
+      <c r="B155" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
-      <c r="A146" s="15" t="s">
+    <row r="156" spans="1:2">
+      <c r="A156" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B146" s="5">
+      <c r="B156" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
-      <c r="A147" s="15" t="s">
+    <row r="157" spans="1:2">
+      <c r="A157" s="16" t="s">
+        <v>512</v>
+      </c>
+      <c r="B157" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="B147" s="5">
+      <c r="B158" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
-      <c r="A148" s="15" t="s">
+    <row r="159" spans="1:2">
+      <c r="A159" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="B148" s="5">
+      <c r="B159" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
-      <c r="A149" s="15" t="s">
+    <row r="160" spans="1:2">
+      <c r="A160" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="B149" s="5">
+      <c r="B160" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
-      <c r="A150" s="15" t="s">
+    <row r="161" spans="1:2">
+      <c r="A161" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B150" s="5">
+      <c r="B161" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
-      <c r="A151" s="15" t="s">
+    <row r="162" spans="1:2">
+      <c r="A162" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="B151" s="5">
+      <c r="B162" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
-      <c r="A152" s="29" t="s">
+    <row r="163" spans="1:2">
+      <c r="A163" s="16" t="s">
+        <v>523</v>
+      </c>
+      <c r="B163" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="B152" s="5">
+      <c r="B164" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
-      <c r="A153" t="s">
-        <v>466</v>
-      </c>
-      <c r="B153" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2">
-      <c r="A154" s="15" t="s">
+    <row r="165" spans="1:2">
+      <c r="A165" t="s">
+        <v>465</v>
+      </c>
+      <c r="B165" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166" s="16" t="s">
+        <v>514</v>
+      </c>
+      <c r="B166" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="B154" s="5">
+      <c r="B167" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
-      <c r="A155" s="15" t="s">
+    <row r="168" spans="1:2">
+      <c r="A168" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="B155" s="5">
+      <c r="B168" s="5">
         <v>35</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
-      <c r="A156" s="15" t="s">
+    <row r="169" spans="1:2">
+      <c r="A169" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="B156" s="5">
+      <c r="B169" s="5">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:B156">
-    <sortCondition ref="A3:A156"/>
+  <sortState ref="A3:B169">
+    <sortCondition ref="A3:A169"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6047,10 +6319,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B34"/>
+      <selection activeCell="A3" sqref="A3:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15"/>
@@ -6069,271 +6341,287 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>446</v>
-      </c>
-      <c r="B2" s="30">
+        <v>445</v>
+      </c>
+      <c r="B2" s="32">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>447</v>
-      </c>
-      <c r="B3" s="30">
+        <v>446</v>
+      </c>
+      <c r="B3" s="32">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>448</v>
-      </c>
-      <c r="B4" s="30">
+        <v>447</v>
+      </c>
+      <c r="B4" s="32">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>449</v>
-      </c>
-      <c r="B5" s="30">
+        <v>448</v>
+      </c>
+      <c r="B5" s="32">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>450</v>
-      </c>
-      <c r="B6" s="30">
+        <v>449</v>
+      </c>
+      <c r="B6" s="32">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>451</v>
-      </c>
-      <c r="B7" s="30">
-        <v>15</v>
+        <v>525</v>
+      </c>
+      <c r="B7" s="32">
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>469</v>
-      </c>
-      <c r="B8" s="30">
-        <v>12</v>
+        <v>524</v>
+      </c>
+      <c r="B8" s="32">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>452</v>
-      </c>
-      <c r="B9" s="30">
-        <v>12</v>
+        <v>450</v>
+      </c>
+      <c r="B9" s="32">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>499</v>
-      </c>
-      <c r="B10" s="30">
-        <v>80</v>
+        <v>468</v>
+      </c>
+      <c r="B10" s="32">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>194</v>
-      </c>
-      <c r="B11" s="30">
-        <v>100</v>
+        <v>451</v>
+      </c>
+      <c r="B11" s="32">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>470</v>
-      </c>
-      <c r="B12" s="30">
-        <v>1</v>
+        <v>498</v>
+      </c>
+      <c r="B12" s="32">
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>471</v>
-      </c>
-      <c r="B13" s="30">
-        <v>1</v>
+        <v>194</v>
+      </c>
+      <c r="B13" s="32">
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>465</v>
-      </c>
-      <c r="B14" s="30">
+        <v>469</v>
+      </c>
+      <c r="B14" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>498</v>
-      </c>
-      <c r="B15" s="30">
-        <v>10</v>
+        <v>470</v>
+      </c>
+      <c r="B15" s="32">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>453</v>
-      </c>
-      <c r="B16" s="30">
-        <v>10</v>
+        <v>464</v>
+      </c>
+      <c r="B16" s="32">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>467</v>
-      </c>
-      <c r="B17" s="30">
+        <v>497</v>
+      </c>
+      <c r="B17" s="32">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>305</v>
-      </c>
-      <c r="B18" s="30">
-        <v>30</v>
+        <v>452</v>
+      </c>
+      <c r="B18" s="32">
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>492</v>
-      </c>
-      <c r="B19" s="30">
-        <v>5</v>
+        <v>466</v>
+      </c>
+      <c r="B19" s="32">
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>468</v>
-      </c>
-      <c r="B20" s="30">
-        <v>70</v>
+        <v>304</v>
+      </c>
+      <c r="B20" s="32">
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>195</v>
-      </c>
-      <c r="B21" s="30">
-        <v>80</v>
+        <v>491</v>
+      </c>
+      <c r="B21" s="32">
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>491</v>
-      </c>
-      <c r="B22" s="30">
-        <v>80</v>
+        <v>467</v>
+      </c>
+      <c r="B22" s="32">
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>454</v>
-      </c>
-      <c r="B23" s="30">
-        <v>12</v>
+        <v>195</v>
+      </c>
+      <c r="B23" s="32">
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>455</v>
-      </c>
-      <c r="B24" s="30">
-        <v>10</v>
+        <v>490</v>
+      </c>
+      <c r="B24" s="32">
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>456</v>
-      </c>
-      <c r="B25" s="30">
-        <v>15</v>
+        <v>453</v>
+      </c>
+      <c r="B25" s="32">
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>457</v>
-      </c>
-      <c r="B26" s="30">
-        <v>12</v>
+        <v>454</v>
+      </c>
+      <c r="B26" s="32">
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>458</v>
-      </c>
-      <c r="B27" s="30">
-        <v>12</v>
+        <v>455</v>
+      </c>
+      <c r="B27" s="32">
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>459</v>
-      </c>
-      <c r="B28" s="30">
+        <v>456</v>
+      </c>
+      <c r="B28" s="32">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>460</v>
-      </c>
-      <c r="B29" s="30">
-        <v>20</v>
+        <v>457</v>
+      </c>
+      <c r="B29" s="32">
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>461</v>
-      </c>
-      <c r="B30" s="30">
+        <v>458</v>
+      </c>
+      <c r="B30" s="32">
         <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>462</v>
-      </c>
-      <c r="B31" s="30">
-        <v>7</v>
+        <v>459</v>
+      </c>
+      <c r="B31" s="32">
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>463</v>
-      </c>
-      <c r="B32" s="30">
+        <v>460</v>
+      </c>
+      <c r="B32" s="32">
         <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>464</v>
-      </c>
-      <c r="B33" s="30">
-        <v>12</v>
+        <v>461</v>
+      </c>
+      <c r="B33" s="32">
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>466</v>
-      </c>
-      <c r="B34" s="30">
+        <v>462</v>
+      </c>
+      <c r="B34" s="32">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>463</v>
+      </c>
+      <c r="B35" s="32">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>465</v>
+      </c>
+      <c r="B36" s="32">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:B34">
-    <sortCondition ref="A3:A34"/>
+  <sortState ref="A3:B36">
+    <sortCondition ref="A3:A36"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
editado ZAPATILLAS DE REPARACIÓN CILINDROS DE FRENO (JGO PARA 1 GOMA)
</commit_message>
<xml_diff>
--- a/clientes/files/TODITICO_CATÁLOGO.xlsx
+++ b/clientes/files/TODITICO_CATÁLOGO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\Documents\Catálogos Proformas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\Documents\Catálogos Proformas\Este\360 Actual\Clientes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42636F3-92F6-4AAD-972E-1D59CA61DF2D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C8E434-6DC5-486B-908D-4B0F524DE75A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAEWOO TICO" sheetId="1" r:id="rId1"/>
@@ -1397,9 +1397,6 @@
     <t>ZAPATILLAS DE BOMBA DE FRENO (REPARACION)</t>
   </si>
   <si>
-    <t>ZAPATILLAS DE REPARACIÓN CILINDROS DE FRENO</t>
-  </si>
-  <si>
     <t>ZAPATILLAS DE REPARACIÓN DE PINZAS DE FRENO JGO</t>
   </si>
   <si>
@@ -1653,6 +1650,9 @@
   </si>
   <si>
     <t>ACEITE DE CAJA AUTOMÁTICA DEXRON III 5L</t>
+  </si>
+  <si>
+    <t>ZAPATILLAS DE REPARACIÓN CILINDROS DE FRENO (JGO PARA 1 GOMA)</t>
   </si>
 </sst>
 </file>
@@ -2130,8 +2130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B276"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" topLeftCell="A263" workbookViewId="0">
+      <selection activeCell="A275" sqref="A275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15"/>
@@ -2158,7 +2158,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B3" s="2">
         <v>12</v>
@@ -2374,7 +2374,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B30" s="2">
         <v>80</v>
@@ -2398,7 +2398,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B33" s="2">
         <v>50</v>
@@ -2406,7 +2406,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B34" s="2">
         <v>12</v>
@@ -2462,7 +2462,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B41" s="2">
         <v>1</v>
@@ -2470,7 +2470,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B42" s="2">
         <v>1</v>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B43" s="2">
         <v>1</v>
@@ -2486,7 +2486,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B44" s="2">
         <v>10</v>
@@ -2518,7 +2518,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B48" s="2">
         <v>10</v>
@@ -2526,7 +2526,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B49" s="2">
         <v>10</v>
@@ -2734,7 +2734,7 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B75" s="2">
         <v>15</v>
@@ -2742,7 +2742,7 @@
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B76" s="2">
         <v>30</v>
@@ -2806,7 +2806,7 @@
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B84" s="2">
         <v>70</v>
@@ -2838,7 +2838,7 @@
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B88" s="2">
         <v>25</v>
@@ -2902,7 +2902,7 @@
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B96" s="2">
         <v>10</v>
@@ -2958,7 +2958,7 @@
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B103" s="2">
         <v>100</v>
@@ -3046,7 +3046,7 @@
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B114" s="2">
         <v>250</v>
@@ -3102,7 +3102,7 @@
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B121" s="2">
         <v>15</v>
@@ -3302,7 +3302,7 @@
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B146" s="2">
         <v>10</v>
@@ -3310,7 +3310,7 @@
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B147" s="2">
         <v>10</v>
@@ -3406,7 +3406,7 @@
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B159" s="2">
         <v>20</v>
@@ -3422,7 +3422,7 @@
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B161" s="2">
         <v>5</v>
@@ -3534,7 +3534,7 @@
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B175" s="2">
         <v>80</v>
@@ -3726,7 +3726,7 @@
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B199" s="2">
         <v>40</v>
@@ -3974,7 +3974,7 @@
     </row>
     <row r="230" spans="1:2">
       <c r="A230" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B230" s="2">
         <v>15</v>
@@ -3982,7 +3982,7 @@
     </row>
     <row r="231" spans="1:2">
       <c r="A231" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B231" s="2">
         <v>6</v>
@@ -4086,7 +4086,7 @@
     </row>
     <row r="244" spans="1:2">
       <c r="A244" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B244" s="2">
         <v>550</v>
@@ -4182,7 +4182,7 @@
     </row>
     <row r="256" spans="1:2">
       <c r="A256" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B256" s="2">
         <v>10</v>
@@ -4254,7 +4254,7 @@
     </row>
     <row r="265" spans="1:2">
       <c r="A265" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B265" s="2">
         <v>3</v>
@@ -4334,7 +4334,7 @@
     </row>
     <row r="275" spans="1:2">
       <c r="A275" t="s">
-        <v>440</v>
+        <v>525</v>
       </c>
       <c r="B275" s="2">
         <v>10</v>
@@ -4342,7 +4342,7 @@
     </row>
     <row r="276" spans="1:2">
       <c r="A276" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B276" s="2">
         <v>15</v>
@@ -4433,7 +4433,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="7" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B9" s="5">
         <v>80</v>
@@ -4473,7 +4473,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B14" s="5">
         <v>1</v>
@@ -4481,7 +4481,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="7" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B15" s="5">
         <v>1</v>
@@ -4489,7 +4489,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
@@ -4497,7 +4497,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="7" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B17" s="5">
         <v>15</v>
@@ -4529,7 +4529,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="7" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B21" s="5">
         <v>7</v>
@@ -4545,7 +4545,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B23" s="5">
         <v>25</v>
@@ -4553,7 +4553,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="7" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B24" s="5">
         <v>50</v>
@@ -4585,7 +4585,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="7" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B28" s="5">
         <v>15</v>
@@ -4609,7 +4609,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B31" s="12">
         <v>100</v>
@@ -4657,7 +4657,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B37" s="12">
         <v>40</v>
@@ -4793,7 +4793,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="7" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B54" s="5">
         <v>40</v>
@@ -4817,7 +4817,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B57" s="12">
         <v>150</v>
@@ -4865,7 +4865,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="7" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B63" s="5">
         <v>40</v>
@@ -4873,7 +4873,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="7" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B64" s="5">
         <v>20</v>
@@ -4889,7 +4889,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B66" s="5">
         <v>5</v>
@@ -4905,7 +4905,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B68" s="2">
         <v>10</v>
@@ -4913,7 +4913,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="7" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B69" s="5">
         <v>15</v>
@@ -4921,7 +4921,7 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B70" s="5">
         <v>10</v>
@@ -5055,7 +5055,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="16" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B13" s="5">
         <v>80</v>
@@ -5151,7 +5151,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="16" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B25" s="5">
         <v>1</v>
@@ -5159,7 +5159,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="16" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B26" s="5">
         <v>1</v>
@@ -5167,7 +5167,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
@@ -5223,7 +5223,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="16" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B34" s="5">
         <v>7</v>
@@ -5239,7 +5239,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="16" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B36" s="5">
         <v>80</v>
@@ -5247,7 +5247,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="16" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B37" s="5">
         <v>90</v>
@@ -5575,7 +5575,7 @@
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="26" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B78" s="12">
         <v>50</v>
@@ -5631,7 +5631,7 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="16" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B85" s="5">
         <v>15</v>
@@ -5671,7 +5671,7 @@
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="16" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B90" s="5">
         <v>80</v>
@@ -5735,7 +5735,7 @@
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B98" s="5">
         <v>20</v>
@@ -5743,7 +5743,7 @@
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="16" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B99" s="5">
         <v>15</v>
@@ -5751,7 +5751,7 @@
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="16" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B100" s="5">
         <v>15</v>
@@ -5759,7 +5759,7 @@
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="16" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B101" s="5">
         <v>25</v>
@@ -5775,7 +5775,7 @@
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="16" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B103" s="5">
         <v>15</v>
@@ -5903,7 +5903,7 @@
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B119" s="5">
         <v>180</v>
@@ -5975,7 +5975,7 @@
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="26" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B128" s="12">
         <v>150</v>
@@ -6207,7 +6207,7 @@
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B157" s="5">
         <v>40</v>
@@ -6255,7 +6255,7 @@
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="16" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B163" s="5">
         <v>70</v>
@@ -6271,7 +6271,7 @@
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B165" s="2">
         <v>10</v>
@@ -6279,7 +6279,7 @@
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="16" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B166" s="5">
         <v>10</v>
@@ -6321,8 +6321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15"/>
@@ -6341,7 +6341,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B2" s="32">
         <v>12</v>
@@ -6349,7 +6349,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B3" s="32">
         <v>50</v>
@@ -6357,7 +6357,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B4" s="32">
         <v>12</v>
@@ -6365,7 +6365,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B5" s="32">
         <v>50</v>
@@ -6373,7 +6373,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B6" s="32">
         <v>50</v>
@@ -6381,7 +6381,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B7" s="32">
         <v>70</v>
@@ -6389,7 +6389,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B8" s="32">
         <v>50</v>
@@ -6397,7 +6397,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B9" s="32">
         <v>15</v>
@@ -6405,7 +6405,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B10" s="32">
         <v>12</v>
@@ -6413,7 +6413,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B11" s="32">
         <v>12</v>
@@ -6421,7 +6421,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B12" s="32">
         <v>80</v>
@@ -6437,7 +6437,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B14" s="32">
         <v>1</v>
@@ -6445,7 +6445,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B15" s="32">
         <v>1</v>
@@ -6453,7 +6453,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B16" s="32">
         <v>1</v>
@@ -6461,7 +6461,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B17" s="32">
         <v>10</v>
@@ -6469,7 +6469,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B18" s="32">
         <v>10</v>
@@ -6477,7 +6477,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B19" s="32">
         <v>10</v>
@@ -6493,7 +6493,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B21" s="32">
         <v>5</v>
@@ -6501,7 +6501,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B22" s="32">
         <v>70</v>
@@ -6517,7 +6517,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B24" s="32">
         <v>80</v>
@@ -6525,7 +6525,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B25" s="32">
         <v>12</v>
@@ -6533,7 +6533,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B26" s="32">
         <v>10</v>
@@ -6541,7 +6541,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B27" s="32">
         <v>15</v>
@@ -6549,7 +6549,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B28" s="32">
         <v>12</v>
@@ -6557,7 +6557,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B29" s="32">
         <v>12</v>
@@ -6565,7 +6565,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B30" s="32">
         <v>12</v>
@@ -6573,7 +6573,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B31" s="32">
         <v>20</v>
@@ -6581,7 +6581,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B32" s="32">
         <v>12</v>
@@ -6589,7 +6589,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B33" s="32">
         <v>7</v>
@@ -6597,7 +6597,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B34" s="32">
         <v>12</v>
@@ -6605,7 +6605,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B35" s="32">
         <v>12</v>
@@ -6613,7 +6613,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B36" s="32">
         <v>10</v>

</xml_diff>

<commit_message>
Modificado Empresas y Clientes con JGO PARA 1 CILINDRO
</commit_message>
<xml_diff>
--- a/clientes/files/TODITICO_CATÁLOGO.xlsx
+++ b/clientes/files/TODITICO_CATÁLOGO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\Documents\Catálogos Proformas\Este\360 Actual\Clientes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C8E434-6DC5-486B-908D-4B0F524DE75A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44A55A4-FE89-4FFF-AAEB-C69BA59D620A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1652,7 +1652,7 @@
     <t>ACEITE DE CAJA AUTOMÁTICA DEXRON III 5L</t>
   </si>
   <si>
-    <t>ZAPATILLAS DE REPARACIÓN CILINDROS DE FRENO (JGO PARA 1 GOMA)</t>
+    <t>ZAPATILLAS DE REPARACIÓN CILINDROS DE FRENO (JGO PARA UN CILINDRO)</t>
   </si>
 </sst>
 </file>
@@ -4337,7 +4337,7 @@
         <v>525</v>
       </c>
       <c r="B275" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="276" spans="1:2">

</xml_diff>

<commit_message>
Modificado kit juntas motor Picanto 2da y 3ra
</commit_message>
<xml_diff>
--- a/clientes/files/TODITICO_CATÁLOGO.xlsx
+++ b/clientes/files/TODITICO_CATÁLOGO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\Documents\Catálogos Proformas\Este\360 Actual\Clientes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44A55A4-FE89-4FFF-AAEB-C69BA59D620A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E40709-5BB6-4E1A-86D0-5D91131E86E5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAEWOO TICO" sheetId="1" r:id="rId1"/>
@@ -580,9 +580,6 @@
     <t>FILTRO ACEITE PICANTO 2DA</t>
   </si>
   <si>
-    <t>KIT DE JUNTAS DEL MOTOR PICANTO 2DA</t>
-  </si>
-  <si>
     <t xml:space="preserve">MANGUERA DE RADIADOR INFERIOR PICANTO 2DA              </t>
   </si>
   <si>
@@ -1653,6 +1650,9 @@
   </si>
   <si>
     <t>ZAPATILLAS DE REPARACIÓN CILINDROS DE FRENO (JGO PARA UN CILINDRO)</t>
+  </si>
+  <si>
+    <t>KIT DE JUNTAS DEL MOTOR PICANTO 2DA Y 3RA</t>
   </si>
 </sst>
 </file>
@@ -1760,7 +1760,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1852,6 +1852,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -2130,7 +2133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A263" workbookViewId="0">
+    <sheetView topLeftCell="A263" workbookViewId="0">
       <selection activeCell="A275" sqref="A275"/>
     </sheetView>
   </sheetViews>
@@ -2150,7 +2153,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B2" s="2">
         <v>10</v>
@@ -2158,7 +2161,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B3" s="2">
         <v>12</v>
@@ -2166,7 +2169,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B4" s="2">
         <v>15</v>
@@ -2174,7 +2177,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B5" s="2">
         <v>10</v>
@@ -2182,7 +2185,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B6" s="2">
         <v>100</v>
@@ -2190,7 +2193,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B7" s="2">
         <v>120</v>
@@ -2198,7 +2201,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B8" s="2">
         <v>100</v>
@@ -2206,7 +2209,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B9" s="2">
         <v>160</v>
@@ -2214,7 +2217,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B10" s="2">
         <v>35</v>
@@ -2222,7 +2225,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B11" s="2">
         <v>150</v>
@@ -2230,7 +2233,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B12" s="2">
         <v>110</v>
@@ -2238,7 +2241,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B13" s="2">
         <v>15</v>
@@ -2246,7 +2249,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B14" s="2">
         <v>40</v>
@@ -2254,7 +2257,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B15" s="2">
         <v>30</v>
@@ -2262,7 +2265,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B16" s="2">
         <v>3</v>
@@ -2270,7 +2273,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B17" s="2">
         <v>15</v>
@@ -2278,7 +2281,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B18" s="2">
         <v>120</v>
@@ -2286,7 +2289,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B19" s="2">
         <v>50</v>
@@ -2294,7 +2297,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B20" s="2">
         <v>10</v>
@@ -2302,7 +2305,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B21" s="2">
         <v>90</v>
@@ -2310,7 +2313,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B22" s="2">
         <v>35</v>
@@ -2318,7 +2321,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B23" s="2">
         <v>10</v>
@@ -2326,7 +2329,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B24" s="2">
         <v>150</v>
@@ -2334,7 +2337,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B25" s="2">
         <v>120</v>
@@ -2342,7 +2345,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B26" s="2">
         <v>170</v>
@@ -2350,7 +2353,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B27" s="2">
         <v>30</v>
@@ -2358,7 +2361,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B28" s="2">
         <v>60</v>
@@ -2366,7 +2369,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B29" s="2">
         <v>30</v>
@@ -2374,7 +2377,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B30" s="2">
         <v>80</v>
@@ -2382,7 +2385,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B31" s="2">
         <v>100</v>
@@ -2390,7 +2393,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B32" s="2">
         <v>25</v>
@@ -2398,7 +2401,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B33" s="2">
         <v>50</v>
@@ -2406,7 +2409,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B34" s="2">
         <v>12</v>
@@ -2414,7 +2417,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B35" s="2">
         <v>40</v>
@@ -2422,7 +2425,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B36" s="2">
         <v>80</v>
@@ -2430,7 +2433,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B37" s="2">
         <v>45</v>
@@ -2438,7 +2441,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B38" s="2">
         <v>60</v>
@@ -2446,7 +2449,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B39" s="2">
         <v>45</v>
@@ -2454,7 +2457,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B40" s="2">
         <v>20</v>
@@ -2462,7 +2465,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B41" s="2">
         <v>1</v>
@@ -2470,7 +2473,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B42" s="2">
         <v>1</v>
@@ -2478,7 +2481,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B43" s="2">
         <v>1</v>
@@ -2486,7 +2489,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B44" s="2">
         <v>10</v>
@@ -2494,7 +2497,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B45" s="2">
         <v>100</v>
@@ -2502,7 +2505,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B46" s="2">
         <v>15</v>
@@ -2510,7 +2513,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B47" s="2">
         <v>10</v>
@@ -2518,7 +2521,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B48" s="2">
         <v>10</v>
@@ -2526,7 +2529,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B49" s="2">
         <v>10</v>
@@ -2534,7 +2537,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B50" s="2">
         <v>60</v>
@@ -2542,7 +2545,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B51" s="2">
         <v>40</v>
@@ -2550,7 +2553,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B52" s="2">
         <v>20</v>
@@ -2558,7 +2561,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B53" s="2">
         <v>15</v>
@@ -2566,7 +2569,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B54" s="2">
         <v>20</v>
@@ -2574,7 +2577,7 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B55" s="2">
         <v>15</v>
@@ -2582,7 +2585,7 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B56" s="2">
         <v>10</v>
@@ -2590,7 +2593,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B57" s="2">
         <v>5</v>
@@ -2598,7 +2601,7 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B58" s="2">
         <v>15</v>
@@ -2606,7 +2609,7 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B59" s="2">
         <v>10</v>
@@ -2614,7 +2617,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B60" s="2">
         <v>2</v>
@@ -2622,7 +2625,7 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B61" s="2">
         <v>15</v>
@@ -2630,7 +2633,7 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B62" s="2">
         <v>15</v>
@@ -2638,7 +2641,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B63" s="2">
         <v>10</v>
@@ -2646,7 +2649,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B64" s="2">
         <v>10</v>
@@ -2654,7 +2657,7 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B65" s="2">
         <v>7</v>
@@ -2662,7 +2665,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B66" s="2">
         <v>10</v>
@@ -2670,7 +2673,7 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B67" s="2">
         <v>15</v>
@@ -2678,7 +2681,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B68" s="2">
         <v>20</v>
@@ -2686,7 +2689,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B69" s="2">
         <v>25</v>
@@ -2694,7 +2697,7 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B70" s="2">
         <v>20</v>
@@ -2702,7 +2705,7 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B71" s="2">
         <v>45</v>
@@ -2710,7 +2713,7 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B72" s="2">
         <v>25</v>
@@ -2718,7 +2721,7 @@
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B73" s="2">
         <v>25</v>
@@ -2726,7 +2729,7 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B74" s="2">
         <v>10</v>
@@ -2734,7 +2737,7 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B75" s="2">
         <v>15</v>
@@ -2742,7 +2745,7 @@
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B76" s="2">
         <v>30</v>
@@ -2750,7 +2753,7 @@
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B77" s="2">
         <v>50</v>
@@ -2758,7 +2761,7 @@
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B78" s="2">
         <v>70</v>
@@ -2766,7 +2769,7 @@
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B79" s="2">
         <v>100</v>
@@ -2774,7 +2777,7 @@
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B80" s="2">
         <v>350</v>
@@ -2782,7 +2785,7 @@
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B81" s="2">
         <v>10</v>
@@ -2790,7 +2793,7 @@
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B82" s="2">
         <v>300</v>
@@ -2798,7 +2801,7 @@
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B83" s="2">
         <v>50</v>
@@ -2806,7 +2809,7 @@
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B84" s="2">
         <v>70</v>
@@ -2814,7 +2817,7 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B85" s="2">
         <v>50</v>
@@ -2822,7 +2825,7 @@
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B86" s="2">
         <v>80</v>
@@ -2830,7 +2833,7 @@
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B87" s="2">
         <v>25</v>
@@ -2838,7 +2841,7 @@
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B88" s="2">
         <v>25</v>
@@ -2846,7 +2849,7 @@
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B89" s="2">
         <v>25</v>
@@ -2854,7 +2857,7 @@
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B90" s="2">
         <v>35</v>
@@ -2862,7 +2865,7 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B91" s="2">
         <v>70</v>
@@ -2870,7 +2873,7 @@
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B92" s="2">
         <v>50</v>
@@ -2878,7 +2881,7 @@
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B93" s="2">
         <v>120</v>
@@ -2886,7 +2889,7 @@
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B94" s="2">
         <v>30</v>
@@ -2894,7 +2897,7 @@
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B95" s="2">
         <v>60</v>
@@ -2902,7 +2905,7 @@
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B96" s="2">
         <v>10</v>
@@ -2910,7 +2913,7 @@
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B97" s="2">
         <v>20</v>
@@ -2918,7 +2921,7 @@
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B98" s="2">
         <v>15</v>
@@ -2926,7 +2929,7 @@
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B99" s="2">
         <v>20</v>
@@ -2934,7 +2937,7 @@
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B100" s="2">
         <v>60</v>
@@ -2942,7 +2945,7 @@
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B101" s="2">
         <v>150</v>
@@ -2950,7 +2953,7 @@
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B102" s="2">
         <v>40</v>
@@ -2958,7 +2961,7 @@
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B103" s="2">
         <v>100</v>
@@ -2966,7 +2969,7 @@
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B104" s="2">
         <v>25</v>
@@ -2974,7 +2977,7 @@
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B105" s="2">
         <v>450</v>
@@ -2982,7 +2985,7 @@
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B106" s="2">
         <v>180</v>
@@ -2990,7 +2993,7 @@
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B107" s="2">
         <v>10</v>
@@ -2998,7 +3001,7 @@
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B108" s="2">
         <v>30</v>
@@ -3006,7 +3009,7 @@
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B109" s="2">
         <v>30</v>
@@ -3014,7 +3017,7 @@
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B110" s="2">
         <v>60</v>
@@ -3022,7 +3025,7 @@
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B111" s="2">
         <v>120</v>
@@ -3030,7 +3033,7 @@
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B112" s="2">
         <v>25</v>
@@ -3038,7 +3041,7 @@
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B113" s="2">
         <v>80</v>
@@ -3046,7 +3049,7 @@
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B114" s="2">
         <v>250</v>
@@ -3062,7 +3065,7 @@
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B116" s="2">
         <v>20</v>
@@ -3070,7 +3073,7 @@
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B117" s="2">
         <v>15</v>
@@ -3078,7 +3081,7 @@
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B118" s="2">
         <v>50</v>
@@ -3086,7 +3089,7 @@
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B119" s="2">
         <v>60</v>
@@ -3094,7 +3097,7 @@
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B120" s="2">
         <v>100</v>
@@ -3102,7 +3105,7 @@
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B121" s="2">
         <v>15</v>
@@ -3110,7 +3113,7 @@
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B122" s="2">
         <v>50</v>
@@ -3118,7 +3121,7 @@
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B123" s="2">
         <v>70</v>
@@ -3126,7 +3129,7 @@
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B124" s="2">
         <v>10</v>
@@ -3134,7 +3137,7 @@
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B125" s="2">
         <v>10</v>
@@ -3142,7 +3145,7 @@
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B126" s="2">
         <v>10</v>
@@ -3150,7 +3153,7 @@
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B127" s="2">
         <v>30</v>
@@ -3158,7 +3161,7 @@
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B128" s="2">
         <v>90</v>
@@ -3166,7 +3169,7 @@
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B129" s="2">
         <v>50</v>
@@ -3174,7 +3177,7 @@
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B130" s="2">
         <v>10</v>
@@ -3182,7 +3185,7 @@
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B131" s="2">
         <v>30</v>
@@ -3190,7 +3193,7 @@
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B132" s="2">
         <v>120</v>
@@ -3198,7 +3201,7 @@
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B133" s="2">
         <v>15</v>
@@ -3206,7 +3209,7 @@
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B134" s="2">
         <v>70</v>
@@ -3214,7 +3217,7 @@
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B135" s="2">
         <v>20</v>
@@ -3222,7 +3225,7 @@
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B136" s="2">
         <v>5</v>
@@ -3230,7 +3233,7 @@
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B137" s="2">
         <v>100</v>
@@ -3238,7 +3241,7 @@
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B138" s="2">
         <v>60</v>
@@ -3246,7 +3249,7 @@
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B139" s="2">
         <v>30</v>
@@ -3254,7 +3257,7 @@
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B140" s="2">
         <v>100</v>
@@ -3262,7 +3265,7 @@
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B141" s="2">
         <v>30</v>
@@ -3270,7 +3273,7 @@
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B142" s="2">
         <v>10</v>
@@ -3278,7 +3281,7 @@
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B143" s="2">
         <v>15</v>
@@ -3286,7 +3289,7 @@
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B144" s="2">
         <v>30</v>
@@ -3294,7 +3297,7 @@
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B145" s="2">
         <v>10</v>
@@ -3302,7 +3305,7 @@
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B146" s="2">
         <v>10</v>
@@ -3310,7 +3313,7 @@
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B147" s="2">
         <v>10</v>
@@ -3318,7 +3321,7 @@
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B148" s="2">
         <v>20</v>
@@ -3326,7 +3329,7 @@
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B149" s="2">
         <v>2</v>
@@ -3334,7 +3337,7 @@
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B150" s="2">
         <v>20</v>
@@ -3342,7 +3345,7 @@
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B151" s="2">
         <v>50</v>
@@ -3350,7 +3353,7 @@
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B152" s="2">
         <v>40</v>
@@ -3358,7 +3361,7 @@
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B153" s="2">
         <v>90</v>
@@ -3366,7 +3369,7 @@
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B154" s="2">
         <v>12</v>
@@ -3374,7 +3377,7 @@
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B155" s="2">
         <v>15</v>
@@ -3382,7 +3385,7 @@
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B156" s="2">
         <v>550</v>
@@ -3390,7 +3393,7 @@
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B157" s="2">
         <v>6</v>
@@ -3398,7 +3401,7 @@
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B158" s="2">
         <v>10</v>
@@ -3406,7 +3409,7 @@
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B159" s="2">
         <v>20</v>
@@ -3414,7 +3417,7 @@
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B160" s="2">
         <v>15</v>
@@ -3422,7 +3425,7 @@
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B161" s="2">
         <v>5</v>
@@ -3430,7 +3433,7 @@
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B162" s="2">
         <v>15</v>
@@ -3438,7 +3441,7 @@
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B163" s="2">
         <v>70</v>
@@ -3446,7 +3449,7 @@
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B164" s="2">
         <v>10</v>
@@ -3454,7 +3457,7 @@
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B165" s="2">
         <v>10</v>
@@ -3462,7 +3465,7 @@
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B166" s="2">
         <v>20</v>
@@ -3470,7 +3473,7 @@
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B167" s="2">
         <v>10</v>
@@ -3478,7 +3481,7 @@
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B168" s="2">
         <v>10</v>
@@ -3486,7 +3489,7 @@
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B169" s="2">
         <v>10</v>
@@ -3494,7 +3497,7 @@
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B170" s="2">
         <v>50</v>
@@ -3502,7 +3505,7 @@
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B171" s="2">
         <v>30</v>
@@ -3510,7 +3513,7 @@
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B172" s="2">
         <v>7</v>
@@ -3518,7 +3521,7 @@
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B173" s="2">
         <v>280</v>
@@ -3526,7 +3529,7 @@
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B174" s="2">
         <v>150</v>
@@ -3534,7 +3537,7 @@
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B175" s="2">
         <v>80</v>
@@ -3542,7 +3545,7 @@
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B176" s="2">
         <v>30</v>
@@ -3550,7 +3553,7 @@
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B177" s="2">
         <v>150</v>
@@ -3558,7 +3561,7 @@
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B178" s="2">
         <v>10</v>
@@ -3566,7 +3569,7 @@
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B179" s="2">
         <v>10</v>
@@ -3574,7 +3577,7 @@
     </row>
     <row r="180" spans="1:2">
       <c r="A180" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B180" s="2">
         <v>20</v>
@@ -3582,7 +3585,7 @@
     </row>
     <row r="181" spans="1:2">
       <c r="A181" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B181" s="2">
         <v>100</v>
@@ -3590,7 +3593,7 @@
     </row>
     <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B182" s="2">
         <v>120</v>
@@ -3598,7 +3601,7 @@
     </row>
     <row r="183" spans="1:2">
       <c r="A183" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B183" s="2">
         <v>300</v>
@@ -3606,7 +3609,7 @@
     </row>
     <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B184" s="2">
         <v>160</v>
@@ -3614,7 +3617,7 @@
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B185" s="2">
         <v>110</v>
@@ -3622,7 +3625,7 @@
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B186" s="2">
         <v>160</v>
@@ -3630,7 +3633,7 @@
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B187" s="2">
         <v>30</v>
@@ -3638,7 +3641,7 @@
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B188" s="2">
         <v>170</v>
@@ -3646,7 +3649,7 @@
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B189" s="2">
         <v>80</v>
@@ -3654,7 +3657,7 @@
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B190" s="2">
         <v>220</v>
@@ -3662,7 +3665,7 @@
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B191" s="2">
         <v>90</v>
@@ -3670,7 +3673,7 @@
     </row>
     <row r="192" spans="1:2">
       <c r="A192" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B192" s="2">
         <v>25</v>
@@ -3678,7 +3681,7 @@
     </row>
     <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B193" s="2">
         <v>70</v>
@@ -3686,7 +3689,7 @@
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B194" s="2">
         <v>25</v>
@@ -3694,7 +3697,7 @@
     </row>
     <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B195" s="2">
         <v>10</v>
@@ -3702,7 +3705,7 @@
     </row>
     <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B196" s="2">
         <v>30</v>
@@ -3710,7 +3713,7 @@
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B197" s="2">
         <v>30</v>
@@ -3718,7 +3721,7 @@
     </row>
     <row r="198" spans="1:2">
       <c r="A198" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B198" s="2">
         <v>60</v>
@@ -3726,7 +3729,7 @@
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B199" s="2">
         <v>40</v>
@@ -3734,7 +3737,7 @@
     </row>
     <row r="200" spans="1:2">
       <c r="A200" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B200" s="2">
         <v>30</v>
@@ -3742,7 +3745,7 @@
     </row>
     <row r="201" spans="1:2">
       <c r="A201" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B201" s="2">
         <v>20</v>
@@ -3750,7 +3753,7 @@
     </row>
     <row r="202" spans="1:2">
       <c r="A202" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B202" s="2">
         <v>20</v>
@@ -3758,7 +3761,7 @@
     </row>
     <row r="203" spans="1:2">
       <c r="A203" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B203" s="2">
         <v>150</v>
@@ -3766,7 +3769,7 @@
     </row>
     <row r="204" spans="1:2">
       <c r="A204" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B204" s="2">
         <v>350</v>
@@ -3774,7 +3777,7 @@
     </row>
     <row r="205" spans="1:2">
       <c r="A205" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B205" s="2">
         <v>20</v>
@@ -3782,7 +3785,7 @@
     </row>
     <row r="206" spans="1:2">
       <c r="A206" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B206" s="2">
         <v>20</v>
@@ -3790,7 +3793,7 @@
     </row>
     <row r="207" spans="1:2">
       <c r="A207" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B207" s="2">
         <v>15</v>
@@ -3798,7 +3801,7 @@
     </row>
     <row r="208" spans="1:2">
       <c r="A208" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B208" s="2">
         <v>30</v>
@@ -3806,7 +3809,7 @@
     </row>
     <row r="209" spans="1:2">
       <c r="A209" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B209" s="2">
         <v>15</v>
@@ -3814,7 +3817,7 @@
     </row>
     <row r="210" spans="1:2">
       <c r="A210" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B210" s="2">
         <v>70</v>
@@ -3822,7 +3825,7 @@
     </row>
     <row r="211" spans="1:2">
       <c r="A211" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B211" s="2">
         <v>40</v>
@@ -3830,7 +3833,7 @@
     </row>
     <row r="212" spans="1:2">
       <c r="A212" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B212" s="2">
         <v>100</v>
@@ -3838,7 +3841,7 @@
     </row>
     <row r="213" spans="1:2">
       <c r="A213" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B213" s="2">
         <v>70</v>
@@ -3846,7 +3849,7 @@
     </row>
     <row r="214" spans="1:2">
       <c r="A214" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B214" s="2">
         <v>15</v>
@@ -3854,7 +3857,7 @@
     </row>
     <row r="215" spans="1:2">
       <c r="A215" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B215" s="2">
         <v>130</v>
@@ -3862,7 +3865,7 @@
     </row>
     <row r="216" spans="1:2">
       <c r="A216" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B216" s="2">
         <v>200</v>
@@ -3870,7 +3873,7 @@
     </row>
     <row r="217" spans="1:2">
       <c r="A217" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B217" s="2">
         <v>30</v>
@@ -3878,7 +3881,7 @@
     </row>
     <row r="218" spans="1:2">
       <c r="A218" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B218" s="2">
         <v>15</v>
@@ -3886,7 +3889,7 @@
     </row>
     <row r="219" spans="1:2">
       <c r="A219" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B219" s="2">
         <v>65</v>
@@ -3894,7 +3897,7 @@
     </row>
     <row r="220" spans="1:2">
       <c r="A220" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B220" s="2">
         <v>95</v>
@@ -3902,7 +3905,7 @@
     </row>
     <row r="221" spans="1:2">
       <c r="A221" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B221" s="2">
         <v>10</v>
@@ -3910,7 +3913,7 @@
     </row>
     <row r="222" spans="1:2">
       <c r="A222" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B222" s="2">
         <v>20</v>
@@ -3918,7 +3921,7 @@
     </row>
     <row r="223" spans="1:2">
       <c r="A223" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B223" s="2">
         <v>10</v>
@@ -3926,7 +3929,7 @@
     </row>
     <row r="224" spans="1:2">
       <c r="A224" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B224" s="2">
         <v>10</v>
@@ -3934,7 +3937,7 @@
     </row>
     <row r="225" spans="1:2">
       <c r="A225" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B225" s="2">
         <v>10</v>
@@ -3942,7 +3945,7 @@
     </row>
     <row r="226" spans="1:2">
       <c r="A226" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B226" s="2">
         <v>10</v>
@@ -3950,7 +3953,7 @@
     </row>
     <row r="227" spans="1:2">
       <c r="A227" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B227" s="2">
         <v>15</v>
@@ -3958,7 +3961,7 @@
     </row>
     <row r="228" spans="1:2">
       <c r="A228" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B228" s="2">
         <v>15</v>
@@ -3966,7 +3969,7 @@
     </row>
     <row r="229" spans="1:2">
       <c r="A229" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B229" s="2">
         <v>15</v>
@@ -3974,7 +3977,7 @@
     </row>
     <row r="230" spans="1:2">
       <c r="A230" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B230" s="2">
         <v>15</v>
@@ -3982,7 +3985,7 @@
     </row>
     <row r="231" spans="1:2">
       <c r="A231" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B231" s="2">
         <v>6</v>
@@ -3990,7 +3993,7 @@
     </row>
     <row r="232" spans="1:2">
       <c r="A232" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B232" s="2">
         <v>10</v>
@@ -3998,7 +4001,7 @@
     </row>
     <row r="233" spans="1:2">
       <c r="A233" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B233" s="2">
         <v>150</v>
@@ -4006,7 +4009,7 @@
     </row>
     <row r="234" spans="1:2">
       <c r="A234" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B234" s="2">
         <v>180</v>
@@ -4014,7 +4017,7 @@
     </row>
     <row r="235" spans="1:2">
       <c r="A235" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B235" s="2">
         <v>90</v>
@@ -4022,7 +4025,7 @@
     </row>
     <row r="236" spans="1:2">
       <c r="A236" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B236" s="2">
         <v>30</v>
@@ -4030,7 +4033,7 @@
     </row>
     <row r="237" spans="1:2">
       <c r="A237" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B237" s="2">
         <v>25</v>
@@ -4038,7 +4041,7 @@
     </row>
     <row r="238" spans="1:2">
       <c r="A238" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B238" s="2">
         <v>4</v>
@@ -4046,7 +4049,7 @@
     </row>
     <row r="239" spans="1:2">
       <c r="A239" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B239" s="2">
         <v>75</v>
@@ -4054,7 +4057,7 @@
     </row>
     <row r="240" spans="1:2">
       <c r="A240" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B240" s="2">
         <v>25</v>
@@ -4062,7 +4065,7 @@
     </row>
     <row r="241" spans="1:2">
       <c r="A241" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B241" s="2">
         <v>70</v>
@@ -4070,7 +4073,7 @@
     </row>
     <row r="242" spans="1:2">
       <c r="A242" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B242" s="2">
         <v>15</v>
@@ -4078,7 +4081,7 @@
     </row>
     <row r="243" spans="1:2">
       <c r="A243" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B243" s="2">
         <v>250</v>
@@ -4086,7 +4089,7 @@
     </row>
     <row r="244" spans="1:2">
       <c r="A244" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B244" s="2">
         <v>550</v>
@@ -4094,7 +4097,7 @@
     </row>
     <row r="245" spans="1:2">
       <c r="A245" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B245" s="2">
         <v>25</v>
@@ -4102,7 +4105,7 @@
     </row>
     <row r="246" spans="1:2">
       <c r="A246" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B246" s="2">
         <v>10</v>
@@ -4110,7 +4113,7 @@
     </row>
     <row r="247" spans="1:2">
       <c r="A247" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B247" s="2">
         <v>10</v>
@@ -4118,7 +4121,7 @@
     </row>
     <row r="248" spans="1:2">
       <c r="A248" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B248" s="2">
         <v>15</v>
@@ -4126,7 +4129,7 @@
     </row>
     <row r="249" spans="1:2">
       <c r="A249" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B249" s="2">
         <v>7</v>
@@ -4134,7 +4137,7 @@
     </row>
     <row r="250" spans="1:2">
       <c r="A250" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B250" s="2">
         <v>50</v>
@@ -4142,7 +4145,7 @@
     </row>
     <row r="251" spans="1:2">
       <c r="A251" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B251" s="2">
         <v>5</v>
@@ -4150,7 +4153,7 @@
     </row>
     <row r="252" spans="1:2">
       <c r="A252" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B252" s="2">
         <v>5</v>
@@ -4158,7 +4161,7 @@
     </row>
     <row r="253" spans="1:2">
       <c r="A253" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B253" s="2">
         <v>5</v>
@@ -4166,7 +4169,7 @@
     </row>
     <row r="254" spans="1:2">
       <c r="A254" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B254" s="2">
         <v>7</v>
@@ -4174,7 +4177,7 @@
     </row>
     <row r="255" spans="1:2">
       <c r="A255" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B255" s="2">
         <v>20</v>
@@ -4182,7 +4185,7 @@
     </row>
     <row r="256" spans="1:2">
       <c r="A256" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B256" s="2">
         <v>10</v>
@@ -4190,7 +4193,7 @@
     </row>
     <row r="257" spans="1:2">
       <c r="A257" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B257" s="2">
         <v>15</v>
@@ -4198,7 +4201,7 @@
     </row>
     <row r="258" spans="1:2">
       <c r="A258" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B258" s="2">
         <v>5</v>
@@ -4206,7 +4209,7 @@
     </row>
     <row r="259" spans="1:2">
       <c r="A259" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B259" s="2">
         <v>7</v>
@@ -4214,7 +4217,7 @@
     </row>
     <row r="260" spans="1:2">
       <c r="A260" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B260" s="2">
         <v>10</v>
@@ -4222,7 +4225,7 @@
     </row>
     <row r="261" spans="1:2">
       <c r="A261" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B261" s="2">
         <v>2</v>
@@ -4230,7 +4233,7 @@
     </row>
     <row r="262" spans="1:2">
       <c r="A262" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B262" s="2">
         <v>5</v>
@@ -4238,7 +4241,7 @@
     </row>
     <row r="263" spans="1:2">
       <c r="A263" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B263" s="2">
         <v>3</v>
@@ -4246,7 +4249,7 @@
     </row>
     <row r="264" spans="1:2">
       <c r="A264" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B264" s="2">
         <v>4</v>
@@ -4254,7 +4257,7 @@
     </row>
     <row r="265" spans="1:2">
       <c r="A265" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B265" s="2">
         <v>3</v>
@@ -4262,7 +4265,7 @@
     </row>
     <row r="266" spans="1:2">
       <c r="A266" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B266" s="2">
         <v>2</v>
@@ -4270,7 +4273,7 @@
     </row>
     <row r="267" spans="1:2">
       <c r="A267" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B267" s="2">
         <v>20</v>
@@ -4278,7 +4281,7 @@
     </row>
     <row r="268" spans="1:2">
       <c r="A268" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B268" s="2">
         <v>25</v>
@@ -4286,7 +4289,7 @@
     </row>
     <row r="269" spans="1:2">
       <c r="A269" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B269" s="2">
         <v>45</v>
@@ -4294,7 +4297,7 @@
     </row>
     <row r="270" spans="1:2">
       <c r="A270" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B270" s="2">
         <v>15</v>
@@ -4302,7 +4305,7 @@
     </row>
     <row r="271" spans="1:2">
       <c r="A271" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B271" s="2">
         <v>60</v>
@@ -4310,7 +4313,7 @@
     </row>
     <row r="272" spans="1:2">
       <c r="A272" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B272" s="2">
         <v>100</v>
@@ -4318,7 +4321,7 @@
     </row>
     <row r="273" spans="1:2">
       <c r="A273" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B273" s="2">
         <v>35</v>
@@ -4326,7 +4329,7 @@
     </row>
     <row r="274" spans="1:2">
       <c r="A274" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B274" s="2">
         <v>10</v>
@@ -4334,7 +4337,7 @@
     </row>
     <row r="275" spans="1:2">
       <c r="A275" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B275" s="2">
         <v>5</v>
@@ -4342,7 +4345,7 @@
     </row>
     <row r="276" spans="1:2">
       <c r="A276" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B276" s="2">
         <v>15</v>
@@ -4393,7 +4396,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B4" s="5">
         <v>120</v>
@@ -4433,7 +4436,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="7" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B9" s="5">
         <v>80</v>
@@ -4441,7 +4444,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B10" s="5">
         <v>100</v>
@@ -4473,7 +4476,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="7" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B14" s="5">
         <v>1</v>
@@ -4481,7 +4484,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B15" s="5">
         <v>1</v>
@@ -4489,7 +4492,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
@@ -4497,7 +4500,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B17" s="5">
         <v>15</v>
@@ -4529,7 +4532,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="7" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B21" s="5">
         <v>7</v>
@@ -4545,7 +4548,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B23" s="5">
         <v>25</v>
@@ -4553,7 +4556,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="7" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B24" s="5">
         <v>50</v>
@@ -4585,7 +4588,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B28" s="5">
         <v>15</v>
@@ -4609,7 +4612,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B31" s="12">
         <v>100</v>
@@ -4657,7 +4660,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B37" s="12">
         <v>40</v>
@@ -4697,7 +4700,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B42" s="5">
         <v>80</v>
@@ -4793,7 +4796,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="7" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B54" s="5">
         <v>40</v>
@@ -4817,7 +4820,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B57" s="12">
         <v>150</v>
@@ -4849,7 +4852,7 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B61" s="5">
         <v>5</v>
@@ -4865,7 +4868,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="7" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B63" s="5">
         <v>40</v>
@@ -4873,7 +4876,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="7" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B64" s="5">
         <v>20</v>
@@ -4889,7 +4892,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="7" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B66" s="5">
         <v>5</v>
@@ -4905,7 +4908,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B68" s="2">
         <v>10</v>
@@ -4913,7 +4916,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="7" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B69" s="5">
         <v>15</v>
@@ -4921,7 +4924,7 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="7" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B70" s="5">
         <v>10</v>
@@ -4947,8 +4950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B169"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B169"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15"/>
@@ -5007,7 +5010,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B7" s="5">
         <v>180</v>
@@ -5023,7 +5026,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B9" s="5">
         <v>120</v>
@@ -5055,7 +5058,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="16" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B13" s="5">
         <v>80</v>
@@ -5063,7 +5066,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B14" s="5">
         <v>100</v>
@@ -5135,7 +5138,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B23" s="5">
         <v>80</v>
@@ -5151,7 +5154,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="16" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B25" s="5">
         <v>1</v>
@@ -5159,7 +5162,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="16" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B26" s="5">
         <v>1</v>
@@ -5167,7 +5170,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
@@ -5223,7 +5226,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B34" s="5">
         <v>7</v>
@@ -5239,7 +5242,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="16" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B36" s="5">
         <v>80</v>
@@ -5247,7 +5250,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="16" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B37" s="5">
         <v>90</v>
@@ -5575,7 +5578,7 @@
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="26" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B78" s="12">
         <v>50</v>
@@ -5631,7 +5634,7 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="16" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B85" s="5">
         <v>15</v>
@@ -5663,7 +5666,7 @@
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B89" s="5">
         <v>80</v>
@@ -5671,7 +5674,7 @@
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="16" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B90" s="5">
         <v>80</v>
@@ -5695,7 +5698,7 @@
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B93" s="5">
         <v>20</v>
@@ -5726,8 +5729,8 @@
       </c>
     </row>
     <row r="97" spans="1:2">
-      <c r="A97" s="16" t="s">
-        <v>171</v>
+      <c r="A97" s="33" t="s">
+        <v>525</v>
       </c>
       <c r="B97" s="5">
         <v>60</v>
@@ -5735,7 +5738,7 @@
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="16" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B98" s="5">
         <v>20</v>
@@ -5743,7 +5746,7 @@
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="16" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B99" s="5">
         <v>15</v>
@@ -5751,7 +5754,7 @@
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B100" s="5">
         <v>15</v>
@@ -5759,7 +5762,7 @@
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="16" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B101" s="5">
         <v>25</v>
@@ -5767,7 +5770,7 @@
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B102" s="5">
         <v>10</v>
@@ -5775,7 +5778,7 @@
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="16" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B103" s="5">
         <v>15</v>
@@ -5783,7 +5786,7 @@
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B104" s="5">
         <v>15</v>
@@ -5823,7 +5826,7 @@
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B109" s="5">
         <v>250</v>
@@ -5903,7 +5906,7 @@
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="16" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B119" s="5">
         <v>180</v>
@@ -5911,7 +5914,7 @@
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B120" s="5">
         <v>35</v>
@@ -5919,7 +5922,7 @@
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B121" s="5">
         <v>35</v>
@@ -5935,7 +5938,7 @@
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B123" s="5">
         <v>70</v>
@@ -5943,7 +5946,7 @@
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B124" s="5">
         <v>60</v>
@@ -5951,7 +5954,7 @@
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B125" s="5">
         <v>45</v>
@@ -5967,7 +5970,7 @@
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B127" s="5">
         <v>45</v>
@@ -5975,7 +5978,7 @@
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="26" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B128" s="12">
         <v>150</v>
@@ -5991,7 +5994,7 @@
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B130" s="5">
         <v>150</v>
@@ -6007,7 +6010,7 @@
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B132" s="5">
         <v>140</v>
@@ -6079,7 +6082,7 @@
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B141" s="5">
         <v>5</v>
@@ -6087,7 +6090,7 @@
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B142" s="5">
         <v>7</v>
@@ -6103,7 +6106,7 @@
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B144" s="5">
         <v>5</v>
@@ -6167,7 +6170,7 @@
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B152" s="5">
         <v>35</v>
@@ -6175,7 +6178,7 @@
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B153" s="5">
         <v>35</v>
@@ -6207,7 +6210,7 @@
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B157" s="5">
         <v>40</v>
@@ -6255,7 +6258,7 @@
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="16" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B163" s="5">
         <v>70</v>
@@ -6271,7 +6274,7 @@
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B165" s="2">
         <v>10</v>
@@ -6279,7 +6282,7 @@
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="16" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B166" s="5">
         <v>10</v>
@@ -6295,7 +6298,7 @@
     </row>
     <row r="168" spans="1:2">
       <c r="A168" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B168" s="5">
         <v>35</v>
@@ -6303,7 +6306,7 @@
     </row>
     <row r="169" spans="1:2">
       <c r="A169" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B169" s="5">
         <v>40</v>
@@ -6341,7 +6344,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B2" s="32">
         <v>12</v>
@@ -6349,7 +6352,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B3" s="32">
         <v>50</v>
@@ -6357,7 +6360,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B4" s="32">
         <v>12</v>
@@ -6365,7 +6368,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B5" s="32">
         <v>50</v>
@@ -6373,7 +6376,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B6" s="32">
         <v>50</v>
@@ -6381,7 +6384,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B7" s="32">
         <v>70</v>
@@ -6389,7 +6392,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B8" s="32">
         <v>50</v>
@@ -6397,7 +6400,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B9" s="32">
         <v>15</v>
@@ -6405,7 +6408,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B10" s="32">
         <v>12</v>
@@ -6413,7 +6416,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B11" s="32">
         <v>12</v>
@@ -6421,7 +6424,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B12" s="32">
         <v>80</v>
@@ -6429,7 +6432,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B13" s="32">
         <v>100</v>
@@ -6437,7 +6440,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B14" s="32">
         <v>1</v>
@@ -6445,7 +6448,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B15" s="32">
         <v>1</v>
@@ -6453,7 +6456,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B16" s="32">
         <v>1</v>
@@ -6461,7 +6464,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B17" s="32">
         <v>10</v>
@@ -6469,7 +6472,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B18" s="32">
         <v>10</v>
@@ -6477,7 +6480,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B19" s="32">
         <v>10</v>
@@ -6485,7 +6488,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B20" s="32">
         <v>30</v>
@@ -6493,7 +6496,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B21" s="32">
         <v>5</v>
@@ -6501,7 +6504,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B22" s="32">
         <v>70</v>
@@ -6509,7 +6512,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B23" s="32">
         <v>80</v>
@@ -6517,7 +6520,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B24" s="32">
         <v>80</v>
@@ -6525,7 +6528,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B25" s="32">
         <v>12</v>
@@ -6533,7 +6536,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B26" s="32">
         <v>10</v>
@@ -6541,7 +6544,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B27" s="32">
         <v>15</v>
@@ -6549,7 +6552,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B28" s="32">
         <v>12</v>
@@ -6557,7 +6560,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B29" s="32">
         <v>12</v>
@@ -6565,7 +6568,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B30" s="32">
         <v>12</v>
@@ -6573,7 +6576,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B31" s="32">
         <v>20</v>
@@ -6581,7 +6584,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B32" s="32">
         <v>12</v>
@@ -6589,7 +6592,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B33" s="32">
         <v>7</v>
@@ -6597,7 +6600,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B34" s="32">
         <v>12</v>
@@ -6605,7 +6608,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B35" s="32">
         <v>12</v>
@@ -6613,7 +6616,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B36" s="32">
         <v>10</v>

</xml_diff>

<commit_message>
Agregado nuevos productos a Empresas y Clientes
</commit_message>
<xml_diff>
--- a/clientes/files/TODITICO_CATÁLOGO.xlsx
+++ b/clientes/files/TODITICO_CATÁLOGO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\Documents\Catálogos Proformas\Este\360 Actual\Clientes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trabajo\Catálogos Proformas\Este\345 Actual\Clientes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E40709-5BB6-4E1A-86D0-5D91131E86E5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D6F561-61BC-471E-819D-A77654688944}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAEWOO TICO" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="541">
   <si>
     <t>DESCRIPCION</t>
   </si>
@@ -932,15 +932,6 @@
     <t>DELCO</t>
   </si>
   <si>
-    <t>DIAFRACMA DE CARBURADOR JGO</t>
-  </si>
-  <si>
-    <t>DIAFRACMA DE HIDROVACK</t>
-  </si>
-  <si>
-    <t>DIAFRACMA DE VACIO DEL CARBURADOR</t>
-  </si>
-  <si>
     <t>DISCO DE EMBRAGUE</t>
   </si>
   <si>
@@ -1653,20 +1644,83 @@
   </si>
   <si>
     <t>KIT DE JUNTAS DEL MOTOR PICANTO 2DA Y 3RA</t>
+  </si>
+  <si>
+    <t>DIAFRAGMA DE CARBURADOR JGO</t>
+  </si>
+  <si>
+    <t>DIAFRAGMA DE HIDROVACK</t>
+  </si>
+  <si>
+    <t>DIAFRAGMA DE VACIO DEL CARBURADOR (VÁLVULA DE ALTA)</t>
+  </si>
+  <si>
+    <t>ADORNO DE LAS PUERTAS EXT C/U</t>
+  </si>
+  <si>
+    <t>ADORNO DE MANILLA EXT C/U</t>
+  </si>
+  <si>
+    <t>ALERON COLA DE PATO MODERNO</t>
+  </si>
+  <si>
+    <t>ARANDELA DE CLAXON</t>
+  </si>
+  <si>
+    <t>FORRO DE TIMON</t>
+  </si>
+  <si>
+    <t>KIT DE BASE DE CARBURADOR</t>
+  </si>
+  <si>
+    <t>MICA DE FARO DEFENSA DELANTERA  SUPER TICO AMBAR</t>
+  </si>
+  <si>
+    <t>MICA DE FARO DEFENSA DELANTERA NORMAL AMBAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TORNILLO DE TUBO DE ESCAPE Y RESORTE </t>
+  </si>
+  <si>
+    <t>TRIANGULO DE PUERTA POST(METAL )</t>
+  </si>
+  <si>
+    <t>VIDRIO DE FARO DIAMANTADO</t>
+  </si>
+  <si>
+    <t>VIDRIO DE FARO NORMAL</t>
+  </si>
+  <si>
+    <t>LLANTAS DE HIERRO JGO</t>
+  </si>
+  <si>
+    <t>PLASTICO EMBELLECEDOR DE CINTURON DE SEGURIDAD</t>
+  </si>
+  <si>
+    <t>PLASTICO LATERAL DEL MALETERO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="[$-280A]General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1723,8 +1777,134 @@
       <sz val="10"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1742,8 +1922,181 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1751,114 +2104,309 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
+    <xf numFmtId="167" fontId="30" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
+  <cellStyles count="46">
+    <cellStyle name="20% - Accent1" xfId="10" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="14" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="18" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="22" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="26" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="30" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="11" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="19" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="23" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="27" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="31" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="12" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="16" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="20" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="24" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="28" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="32" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="9" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="13" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="17" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="21" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="25" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="29" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="3" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="7" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="8" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Excel Built-in Normal" xfId="34" xr:uid="{688960BC-F69C-49B0-8CDB-DE122EA836A3}"/>
+    <cellStyle name="Explanatory Text 2" xfId="43" xr:uid="{BF74F976-326C-465D-A83B-19341F51278D}"/>
+    <cellStyle name="Good" xfId="2" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1 2" xfId="36" xr:uid="{35512690-E337-4424-84E2-85231B3DD88C}"/>
+    <cellStyle name="Heading 2 2" xfId="37" xr:uid="{A31B7674-2027-48CB-881D-281F8DA7106C}"/>
+    <cellStyle name="Heading 3 2" xfId="38" xr:uid="{BD8E1F66-2E87-475C-B836-F098EB1FF038}"/>
+    <cellStyle name="Heading 4 2" xfId="39" xr:uid="{C03D7A95-4AB4-46A8-9B28-E35A5D0CCB4A}"/>
+    <cellStyle name="Input" xfId="5" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell 2" xfId="40" xr:uid="{8CB1EC70-1736-4A8C-8B05-273AC47130F4}"/>
+    <cellStyle name="Millares 2" xfId="45" xr:uid="{8123F2D9-FB29-45A7-A0C8-90489F326596}"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="33" xr:uid="{2EE8B4EC-D36D-4191-B1B1-5D6B79B67CDB}"/>
+    <cellStyle name="Note 2" xfId="42" xr:uid="{05480AC8-7CE6-4493-9059-76695070FEBC}"/>
+    <cellStyle name="Output" xfId="6" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title 2" xfId="35" xr:uid="{ECA6EB64-49AC-4841-8FD4-8054B3948E49}"/>
+    <cellStyle name="Total 2" xfId="44" xr:uid="{32CEC7C7-5959-4220-8408-34D306D749D8}"/>
+    <cellStyle name="Warning Text 2" xfId="41" xr:uid="{58D3DC39-F6BA-4D4D-8C44-D27B2207069F}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2131,16 +2679,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B276"/>
+  <dimension ref="A1:B291"/>
   <sheetViews>
-    <sheetView topLeftCell="A263" workbookViewId="0">
-      <selection activeCell="A275" sqref="A275"/>
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B291"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="88.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="88.54296875" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2161,7 +2709,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B3" s="2">
         <v>12</v>
@@ -2177,463 +2725,463 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>526</v>
       </c>
       <c r="B5" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>527</v>
       </c>
       <c r="B6" s="2">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B7" s="2">
-        <v>120</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B8" s="2">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>203</v>
+        <v>528</v>
       </c>
       <c r="B9" s="2">
-        <v>160</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B10" s="2">
-        <v>35</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B11" s="2">
-        <v>150</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B12" s="2">
-        <v>110</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B13" s="2">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B14" s="2">
-        <v>40</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B15" s="2">
-        <v>30</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B16" s="2">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B17" s="2">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B18" s="2">
-        <v>120</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>213</v>
+        <v>529</v>
       </c>
       <c r="B19" s="2">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B20" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B21" s="2">
-        <v>90</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B22" s="2">
-        <v>35</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B23" s="2">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B24" s="2">
-        <v>150</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B25" s="2">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B26" s="2">
-        <v>170</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B27" s="2">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B28" s="2">
-        <v>60</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="3" t="s">
-        <v>223</v>
+      <c r="A29" t="s">
+        <v>219</v>
       </c>
       <c r="B29" s="2">
-        <v>30</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>496</v>
+        <v>220</v>
       </c>
       <c r="B30" s="2">
-        <v>80</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>193</v>
+        <v>221</v>
       </c>
       <c r="B31" s="2">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B32" s="2">
-        <v>25</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>482</v>
+      <c r="A33" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="B33" s="2">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>470</v>
+        <v>493</v>
       </c>
       <c r="B34" s="2">
-        <v>12</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
       <c r="B35" s="2">
-        <v>40</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B36" s="2">
-        <v>80</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>227</v>
+        <v>479</v>
       </c>
       <c r="B37" s="2">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>228</v>
+        <v>467</v>
       </c>
       <c r="B38" s="2">
-        <v>60</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B39" s="2">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B40" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>467</v>
+        <v>227</v>
       </c>
       <c r="B41" s="2">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>468</v>
+        <v>228</v>
       </c>
       <c r="B42" s="2">
-        <v>1</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>462</v>
+        <v>229</v>
       </c>
       <c r="B43" s="2">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>495</v>
+        <v>230</v>
       </c>
       <c r="B44" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>231</v>
+        <v>464</v>
       </c>
       <c r="B45" s="2">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>232</v>
+        <v>465</v>
       </c>
       <c r="B46" s="2">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>233</v>
+        <v>459</v>
       </c>
       <c r="B47" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="3" t="s">
-        <v>440</v>
+      <c r="A48" t="s">
+        <v>492</v>
       </c>
       <c r="B48" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="3" t="s">
-        <v>441</v>
+      <c r="A49" t="s">
+        <v>231</v>
       </c>
       <c r="B49" s="2">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B50" s="2">
-        <v>60</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B51" s="2">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" t="s">
-        <v>236</v>
+      <c r="A52" s="3" t="s">
+        <v>437</v>
       </c>
       <c r="B52" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" t="s">
-        <v>237</v>
+      <c r="A53" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="B53" s="2">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B54" s="2">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B55" s="2">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B56" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B57" s="2">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B58" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B59" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="B60" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B61" s="2">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B62" s="2">
         <v>15</v>
@@ -2641,7 +3189,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B63" s="2">
         <v>10</v>
@@ -2649,79 +3197,79 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B64" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B65" s="2">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B66" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B67" s="2">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B68" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="B69" s="2">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B70" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B71" s="2">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B72" s="2">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B73" s="2">
         <v>25</v>
@@ -2729,335 +3277,335 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B74" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>480</v>
+        <v>255</v>
       </c>
       <c r="B75" s="2">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>481</v>
+        <v>256</v>
       </c>
       <c r="B76" s="2">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B77" s="2">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B78" s="2">
-        <v>70</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>261</v>
+        <v>477</v>
       </c>
       <c r="B79" s="2">
-        <v>100</v>
+        <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>262</v>
+        <v>478</v>
       </c>
       <c r="B80" s="2">
-        <v>350</v>
+        <v>30</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B81" s="2">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B82" s="2">
-        <v>300</v>
+        <v>70</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B83" s="2">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>471</v>
+        <v>262</v>
       </c>
       <c r="B84" s="2">
-        <v>70</v>
+        <v>350</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B85" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B86" s="2">
-        <v>80</v>
+        <v>300</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B87" s="2">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>487</v>
+        <v>468</v>
       </c>
       <c r="B88" s="2">
-        <v>25</v>
+        <v>70</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B89" s="2">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B90" s="2">
-        <v>35</v>
+        <v>80</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B91" s="2">
-        <v>70</v>
+        <v>25</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>272</v>
+        <v>484</v>
       </c>
       <c r="B92" s="2">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B93" s="2">
-        <v>120</v>
+        <v>25</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B94" s="2">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B95" s="2">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>472</v>
+        <v>272</v>
       </c>
       <c r="B96" s="2">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B97" s="2">
-        <v>20</v>
+        <v>120</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B98" s="2">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B99" s="2">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>279</v>
+        <v>469</v>
       </c>
       <c r="B100" s="2">
-        <v>60</v>
+        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B101" s="2">
-        <v>150</v>
+        <v>20</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B102" s="2">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>497</v>
+        <v>278</v>
       </c>
       <c r="B103" s="2">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B104" s="2">
-        <v>25</v>
+        <v>60</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B105" s="2">
-        <v>450</v>
+        <v>150</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B106" s="2">
-        <v>180</v>
+        <v>40</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>285</v>
+        <v>494</v>
       </c>
       <c r="B107" s="2">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B108" s="2">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B109" s="2">
-        <v>30</v>
+        <v>450</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B110" s="2">
-        <v>60</v>
+        <v>180</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>289</v>
+        <v>523</v>
       </c>
       <c r="B111" s="2">
-        <v>120</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>290</v>
+        <v>524</v>
       </c>
       <c r="B112" s="2">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>292</v>
+        <v>525</v>
       </c>
       <c r="B113" s="2">
-        <v>80</v>
+        <v>30</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>483</v>
+        <v>285</v>
       </c>
       <c r="B114" s="2">
-        <v>250</v>
+        <v>60</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>16</v>
+        <v>286</v>
       </c>
       <c r="B115" s="2">
         <v>120</v>
@@ -3065,47 +3613,47 @@
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="B116" s="2">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B117" s="2">
-        <v>15</v>
+        <v>80</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>294</v>
+        <v>480</v>
       </c>
       <c r="B118" s="2">
-        <v>50</v>
+        <v>250</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>295</v>
+        <v>16</v>
       </c>
       <c r="B119" s="2">
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B120" s="2">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="121" spans="1:2">
-      <c r="A121" s="3" t="s">
-        <v>442</v>
+      <c r="A121" t="s">
+        <v>288</v>
       </c>
       <c r="B121" s="2">
         <v>15</v>
@@ -3113,7 +3661,7 @@
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B122" s="2">
         <v>50</v>
@@ -3121,63 +3669,63 @@
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B123" s="2">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B124" s="2">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="125" spans="1:2">
-      <c r="A125" t="s">
-        <v>300</v>
+      <c r="A125" s="3" t="s">
+        <v>439</v>
       </c>
       <c r="B125" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="B126" s="2">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="B127" s="2">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="B128" s="2">
-        <v>90</v>
+        <v>10</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="B129" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B130" s="2">
         <v>10</v>
@@ -3185,7 +3733,7 @@
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B131" s="2">
         <v>30</v>
@@ -3193,103 +3741,103 @@
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B132" s="2">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B133" s="2">
-        <v>15</v>
+        <v>50</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="B134" s="2">
-        <v>70</v>
+        <v>10</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="B135" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>311</v>
+        <v>530</v>
       </c>
       <c r="B136" s="2">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="B137" s="2">
-        <v>100</v>
+        <v>120</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="B138" s="2">
-        <v>60</v>
+        <v>15</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="B139" s="2">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="B140" s="2">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B141" s="2">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="B142" s="2">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B143" s="2">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="B144" s="2">
         <v>30</v>
@@ -3297,23 +3845,23 @@
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="B145" s="2">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>485</v>
+        <v>313</v>
       </c>
       <c r="B146" s="2">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>486</v>
+        <v>314</v>
       </c>
       <c r="B147" s="2">
         <v>10</v>
@@ -3321,143 +3869,143 @@
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="B148" s="2">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="B149" s="2">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B150" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>324</v>
+        <v>482</v>
       </c>
       <c r="B151" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>325</v>
+        <v>483</v>
       </c>
       <c r="B152" s="2">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B153" s="2">
-        <v>90</v>
+        <v>20</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="B154" s="2">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="B155" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="B156" s="2">
-        <v>550</v>
+        <v>50</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="B157" s="2">
-        <v>6</v>
+        <v>40</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>331</v>
+        <v>531</v>
       </c>
       <c r="B158" s="2">
-        <v>10</v>
+        <v>180</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>473</v>
+        <v>323</v>
       </c>
       <c r="B159" s="2">
-        <v>20</v>
+        <v>90</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="B160" s="2">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>474</v>
+        <v>325</v>
       </c>
       <c r="B161" s="2">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>333</v>
+        <v>538</v>
       </c>
       <c r="B162" s="2">
-        <v>15</v>
+        <v>400</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="B163" s="2">
-        <v>70</v>
+        <v>550</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B164" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="B165" s="2">
         <v>10</v>
@@ -3465,7 +4013,7 @@
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>337</v>
+        <v>470</v>
       </c>
       <c r="B166" s="2">
         <v>20</v>
@@ -3473,239 +4021,239 @@
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B167" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>339</v>
+        <v>471</v>
       </c>
       <c r="B168" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="B169" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="B170" s="2">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="B171" s="2">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="B172" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="B173" s="2">
-        <v>280</v>
+        <v>20</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="B174" s="2">
-        <v>150</v>
+        <v>10</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>475</v>
+        <v>336</v>
       </c>
       <c r="B175" s="2">
-        <v>80</v>
+        <v>10</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="B176" s="2">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="B177" s="2">
-        <v>150</v>
+        <v>50</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>348</v>
+        <v>532</v>
       </c>
       <c r="B178" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>349</v>
+        <v>533</v>
       </c>
       <c r="B179" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="B180" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="B181" s="2">
-        <v>100</v>
+        <v>7</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="B182" s="2">
-        <v>120</v>
+        <v>280</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="B183" s="2">
-        <v>300</v>
+        <v>150</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>354</v>
+        <v>472</v>
       </c>
       <c r="B184" s="2">
-        <v>160</v>
+        <v>80</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="B185" s="2">
-        <v>110</v>
+        <v>30</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="B186" s="2">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="B187" s="2">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="B188" s="2">
-        <v>170</v>
+        <v>10</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="B189" s="2">
-        <v>80</v>
+        <v>20</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="B190" s="2">
-        <v>220</v>
+        <v>100</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="B191" s="2">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="B192" s="2">
-        <v>25</v>
+        <v>300</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="B193" s="2">
-        <v>70</v>
+        <v>160</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="B194" s="2">
-        <v>25</v>
+        <v>110</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="B195" s="2">
-        <v>10</v>
+        <v>160</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="B196" s="2">
         <v>30</v>
@@ -3713,95 +4261,95 @@
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="B197" s="2">
-        <v>30</v>
+        <v>170</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="B198" s="2">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>477</v>
+        <v>357</v>
       </c>
       <c r="B199" s="2">
-        <v>40</v>
+        <v>220</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c r="B200" s="2">
-        <v>30</v>
+        <v>90</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="B201" s="2">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="B202" s="2">
-        <v>20</v>
+        <v>70</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="B203" s="2">
-        <v>150</v>
+        <v>25</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="B204" s="2">
-        <v>350</v>
+        <v>10</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" t="s">
-        <v>374</v>
+        <v>539</v>
       </c>
       <c r="B205" s="2">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" t="s">
-        <v>375</v>
+        <v>540</v>
       </c>
       <c r="B206" s="2">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="B207" s="2">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
       <c r="B208" s="2">
         <v>30</v>
@@ -3809,79 +4357,79 @@
     </row>
     <row r="209" spans="1:2">
       <c r="A209" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="B209" s="2">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" t="s">
-        <v>379</v>
+        <v>474</v>
       </c>
       <c r="B210" s="2">
-        <v>70</v>
+        <v>40</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
       <c r="B211" s="2">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="B212" s="2">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
       <c r="B213" s="2">
-        <v>70</v>
+        <v>20</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="B214" s="2">
-        <v>15</v>
+        <v>150</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="B215" s="2">
-        <v>130</v>
+        <v>350</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="B216" s="2">
-        <v>200</v>
+        <v>20</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
       <c r="B217" s="2">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="B218" s="2">
         <v>15</v>
@@ -3889,87 +4437,87 @@
     </row>
     <row r="219" spans="1:2">
       <c r="A219" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
       <c r="B219" s="2">
-        <v>65</v>
+        <v>30</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
       <c r="B220" s="2">
-        <v>95</v>
+        <v>15</v>
       </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
       <c r="B221" s="2">
-        <v>10</v>
+        <v>70</v>
       </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="B222" s="2">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="B223" s="2">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
       <c r="B224" s="2">
-        <v>10</v>
+        <v>70</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="B225" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="B226" s="2">
-        <v>10</v>
+        <v>130</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="B227" s="2">
-        <v>15</v>
+        <v>200</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="B228" s="2">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="B229" s="2">
         <v>15</v>
@@ -3977,23 +4525,23 @@
     </row>
     <row r="230" spans="1:2">
       <c r="A230" t="s">
-        <v>478</v>
+        <v>385</v>
       </c>
       <c r="B230" s="2">
-        <v>15</v>
+        <v>65</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231" t="s">
-        <v>479</v>
+        <v>386</v>
       </c>
       <c r="B231" s="2">
-        <v>6</v>
+        <v>95</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="B232" s="2">
         <v>10</v>
@@ -4001,239 +4549,239 @@
     </row>
     <row r="233" spans="1:2">
       <c r="A233" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="B233" s="2">
-        <v>150</v>
+        <v>20</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="B234" s="2">
-        <v>180</v>
+        <v>10</v>
       </c>
     </row>
     <row r="235" spans="1:2">
       <c r="A235" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
       <c r="B235" s="2">
-        <v>90</v>
+        <v>10</v>
       </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
       <c r="B236" s="2">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
       <c r="B237" s="2">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
       <c r="B238" s="2">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
       <c r="B239" s="2">
-        <v>75</v>
+        <v>15</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="B240" s="2">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241" t="s">
-        <v>408</v>
+        <v>475</v>
       </c>
       <c r="B241" s="2">
-        <v>70</v>
+        <v>15</v>
       </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242" t="s">
-        <v>409</v>
+        <v>476</v>
       </c>
       <c r="B242" s="2">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="B243" s="2">
-        <v>250</v>
+        <v>10</v>
       </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244" t="s">
-        <v>469</v>
+        <v>397</v>
       </c>
       <c r="B244" s="2">
-        <v>550</v>
+        <v>150</v>
       </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="B245" s="2">
-        <v>25</v>
+        <v>180</v>
       </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
       <c r="B246" s="2">
-        <v>10</v>
+        <v>90</v>
       </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="B247" s="2">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="B248" s="2">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="B249" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="B250" s="2">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="251" spans="1:2">
       <c r="A251" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
       <c r="B251" s="2">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" t="s">
-        <v>418</v>
+        <v>405</v>
       </c>
       <c r="B252" s="2">
-        <v>5</v>
+        <v>70</v>
       </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
       <c r="B253" s="2">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="254" spans="1:2">
       <c r="A254" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="B254" s="2">
-        <v>7</v>
+        <v>250</v>
       </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255" t="s">
-        <v>421</v>
+        <v>466</v>
       </c>
       <c r="B255" s="2">
-        <v>20</v>
+        <v>550</v>
       </c>
     </row>
     <row r="256" spans="1:2">
       <c r="A256" t="s">
-        <v>463</v>
+        <v>408</v>
       </c>
       <c r="B256" s="2">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="257" spans="1:2">
       <c r="A257" t="s">
-        <v>422</v>
+        <v>409</v>
       </c>
       <c r="B257" s="2">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="258" spans="1:2">
       <c r="A258" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="B258" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="259" spans="1:2">
       <c r="A259" t="s">
-        <v>424</v>
+        <v>411</v>
       </c>
       <c r="B259" s="2">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
       <c r="B260" s="2">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="261" spans="1:2">
       <c r="A261" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="B261" s="2">
-        <v>2</v>
+        <v>50</v>
       </c>
     </row>
     <row r="262" spans="1:2">
       <c r="A262" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="B262" s="2">
         <v>5</v>
@@ -4241,117 +4789,240 @@
     </row>
     <row r="263" spans="1:2">
       <c r="A263" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="B263" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="264" spans="1:2">
       <c r="A264" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
       <c r="B264" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="265" spans="1:2">
       <c r="A265" t="s">
-        <v>476</v>
+        <v>417</v>
       </c>
       <c r="B265" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="266" spans="1:2">
       <c r="A266" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="B266" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="267" spans="1:2">
       <c r="A267" t="s">
-        <v>431</v>
+        <v>460</v>
       </c>
       <c r="B267" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="268" spans="1:2">
       <c r="A268" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
       <c r="B268" s="2">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="269" spans="1:2">
       <c r="A269" t="s">
-        <v>433</v>
+        <v>420</v>
       </c>
       <c r="B269" s="2">
-        <v>45</v>
+        <v>5</v>
       </c>
     </row>
     <row r="270" spans="1:2">
       <c r="A270" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="B270" s="2">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="271" spans="1:2">
       <c r="A271" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
       <c r="B271" s="2">
-        <v>60</v>
+        <v>10</v>
       </c>
     </row>
     <row r="272" spans="1:2">
       <c r="A272" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
       <c r="B272" s="2">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
       <c r="B273" s="2">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="274" spans="1:2">
       <c r="A274" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
       <c r="B274" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="275" spans="1:2">
       <c r="A275" t="s">
-        <v>524</v>
+        <v>426</v>
       </c>
       <c r="B275" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="276" spans="1:2">
       <c r="A276" t="s">
-        <v>439</v>
+        <v>473</v>
       </c>
       <c r="B276" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2">
+      <c r="A277" t="s">
+        <v>534</v>
+      </c>
+      <c r="B277" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2">
+      <c r="A278" t="s">
+        <v>427</v>
+      </c>
+      <c r="B278" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2">
+      <c r="A279" t="s">
+        <v>535</v>
+      </c>
+      <c r="B279" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2">
+      <c r="A280" t="s">
+        <v>428</v>
+      </c>
+      <c r="B280" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2">
+      <c r="A281" t="s">
+        <v>429</v>
+      </c>
+      <c r="B281" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2">
+      <c r="A282" t="s">
+        <v>430</v>
+      </c>
+      <c r="B282" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2">
+      <c r="A283" t="s">
+        <v>431</v>
+      </c>
+      <c r="B283" s="2">
         <v>15</v>
       </c>
     </row>
+    <row r="284" spans="1:2">
+      <c r="A284" t="s">
+        <v>432</v>
+      </c>
+      <c r="B284" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2">
+      <c r="A285" t="s">
+        <v>433</v>
+      </c>
+      <c r="B285" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2">
+      <c r="A286" t="s">
+        <v>536</v>
+      </c>
+      <c r="B286" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2">
+      <c r="A287" t="s">
+        <v>537</v>
+      </c>
+      <c r="B287" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2">
+      <c r="A288" t="s">
+        <v>434</v>
+      </c>
+      <c r="B288" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2">
+      <c r="A289" t="s">
+        <v>435</v>
+      </c>
+      <c r="B289" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2">
+      <c r="A290" t="s">
+        <v>521</v>
+      </c>
+      <c r="B290" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2">
+      <c r="A291" t="s">
+        <v>436</v>
+      </c>
+      <c r="B291" s="2">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A2:B291">
+    <sortCondition ref="A2:A291"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4364,7 +5035,7 @@
       <selection activeCell="A3" sqref="A3:B71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
@@ -4436,7 +5107,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="7" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B9" s="5">
         <v>80</v>
@@ -4476,7 +5147,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="7" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B14" s="5">
         <v>1</v>
@@ -4484,7 +5155,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="7" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B15" s="5">
         <v>1</v>
@@ -4492,7 +5163,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
@@ -4500,7 +5171,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="7" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B17" s="5">
         <v>15</v>
@@ -4532,7 +5203,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="7" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B21" s="5">
         <v>7</v>
@@ -4548,7 +5219,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="7" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B23" s="5">
         <v>25</v>
@@ -4556,7 +5227,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="7" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B24" s="5">
         <v>50</v>
@@ -4588,7 +5259,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="7" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B28" s="5">
         <v>15</v>
@@ -4612,7 +5283,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B31" s="12">
         <v>100</v>
@@ -4660,7 +5331,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B37" s="12">
         <v>40</v>
@@ -4796,7 +5467,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="7" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B54" s="5">
         <v>40</v>
@@ -4820,7 +5491,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B57" s="12">
         <v>150</v>
@@ -4868,7 +5539,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="7" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B63" s="5">
         <v>40</v>
@@ -4876,7 +5547,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="7" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B64" s="5">
         <v>20</v>
@@ -4892,7 +5563,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="7" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B66" s="5">
         <v>5</v>
@@ -4908,7 +5579,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B68" s="2">
         <v>10</v>
@@ -4916,7 +5587,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="7" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B69" s="5">
         <v>15</v>
@@ -4924,7 +5595,7 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="7" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B70" s="5">
         <v>10</v>
@@ -4950,13 +5621,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+    <sheetView topLeftCell="A83" workbookViewId="0">
       <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="73.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="73.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5058,7 +5729,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="16" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B13" s="5">
         <v>80</v>
@@ -5154,7 +5825,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="16" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B25" s="5">
         <v>1</v>
@@ -5162,7 +5833,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="16" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B26" s="5">
         <v>1</v>
@@ -5170,7 +5841,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
@@ -5226,7 +5897,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="16" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="B34" s="5">
         <v>7</v>
@@ -5242,7 +5913,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="16" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B36" s="5">
         <v>80</v>
@@ -5250,7 +5921,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="16" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B37" s="5">
         <v>90</v>
@@ -5578,7 +6249,7 @@
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="26" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B78" s="12">
         <v>50</v>
@@ -5634,7 +6305,7 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B85" s="5">
         <v>15</v>
@@ -5674,7 +6345,7 @@
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="16" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B90" s="5">
         <v>80</v>
@@ -5730,7 +6401,7 @@
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="33" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="B97" s="5">
         <v>60</v>
@@ -5738,7 +6409,7 @@
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="16" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="B98" s="5">
         <v>20</v>
@@ -5746,7 +6417,7 @@
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="16" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="B99" s="5">
         <v>15</v>
@@ -5754,7 +6425,7 @@
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="16" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B100" s="5">
         <v>15</v>
@@ -5762,7 +6433,7 @@
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="16" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B101" s="5">
         <v>25</v>
@@ -5778,7 +6449,7 @@
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="16" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B103" s="5">
         <v>15</v>
@@ -5906,7 +6577,7 @@
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="16" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B119" s="5">
         <v>180</v>
@@ -5978,7 +6649,7 @@
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="26" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B128" s="12">
         <v>150</v>
@@ -6210,7 +6881,7 @@
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="16" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B157" s="5">
         <v>40</v>
@@ -6258,7 +6929,7 @@
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="16" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B163" s="5">
         <v>70</v>
@@ -6274,7 +6945,7 @@
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B165" s="2">
         <v>10</v>
@@ -6282,7 +6953,7 @@
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B166" s="5">
         <v>10</v>
@@ -6328,10 +6999,10 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="54.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="54.1796875" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -6344,7 +7015,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B2" s="32">
         <v>12</v>
@@ -6352,7 +7023,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B3" s="32">
         <v>50</v>
@@ -6360,7 +7031,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B4" s="32">
         <v>12</v>
@@ -6368,7 +7039,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B5" s="32">
         <v>50</v>
@@ -6376,7 +7047,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B6" s="32">
         <v>50</v>
@@ -6384,7 +7055,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="B7" s="32">
         <v>70</v>
@@ -6392,7 +7063,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B8" s="32">
         <v>50</v>
@@ -6400,7 +7071,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B9" s="32">
         <v>15</v>
@@ -6408,7 +7079,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B10" s="32">
         <v>12</v>
@@ -6416,7 +7087,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B11" s="32">
         <v>12</v>
@@ -6424,7 +7095,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B12" s="32">
         <v>80</v>
@@ -6440,7 +7111,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B14" s="32">
         <v>1</v>
@@ -6448,7 +7119,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B15" s="32">
         <v>1</v>
@@ -6456,7 +7127,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B16" s="32">
         <v>1</v>
@@ -6464,7 +7135,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B17" s="32">
         <v>10</v>
@@ -6472,7 +7143,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B18" s="32">
         <v>10</v>
@@ -6480,7 +7151,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B19" s="32">
         <v>10</v>
@@ -6488,7 +7159,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B20" s="32">
         <v>30</v>
@@ -6496,7 +7167,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B21" s="32">
         <v>5</v>
@@ -6504,7 +7175,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B22" s="32">
         <v>70</v>
@@ -6520,7 +7191,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B24" s="32">
         <v>80</v>
@@ -6528,7 +7199,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B25" s="32">
         <v>12</v>
@@ -6536,7 +7207,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B26" s="32">
         <v>10</v>
@@ -6544,7 +7215,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B27" s="32">
         <v>15</v>
@@ -6552,7 +7223,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B28" s="32">
         <v>12</v>
@@ -6560,7 +7231,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B29" s="32">
         <v>12</v>
@@ -6568,7 +7239,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B30" s="32">
         <v>12</v>
@@ -6576,7 +7247,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B31" s="32">
         <v>20</v>
@@ -6584,7 +7255,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B32" s="32">
         <v>12</v>
@@ -6592,7 +7263,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B33" s="32">
         <v>7</v>
@@ -6600,7 +7271,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B34" s="32">
         <v>12</v>
@@ -6608,7 +7279,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B35" s="32">
         <v>12</v>
@@ -6616,7 +7287,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B36" s="32">
         <v>10</v>

</xml_diff>

<commit_message>
Actualizado Proforma y Clientes
</commit_message>
<xml_diff>
--- a/clientes/files/TODITICO_CATÁLOGO.xlsx
+++ b/clientes/files/TODITICO_CATÁLOGO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trabajo\Catálogos Proformas\Este\320 Actual\Clientes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD0C86F-BABD-409C-AC68-3C16C4FE6388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD42A0D-F77E-4722-AF1E-3F2639224D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAEWOO TICO" sheetId="1" r:id="rId1"/>
@@ -2671,8 +2671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A159" sqref="A159:B291"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="14.5"/>
@@ -5010,7 +5010,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A291">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B291">
     <sortCondition ref="A2:A291"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5021,8 +5021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="14.5"/>
@@ -5616,8 +5616,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A73">
-    <sortCondition ref="A3:A73"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B73">
+    <sortCondition ref="A2:A73"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5627,8 +5627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B169"/>
   <sheetViews>
-    <sheetView topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="14.5"/>
@@ -6990,8 +6990,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A169">
-    <sortCondition ref="A3:A169"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B169">
+    <sortCondition ref="A2:A169"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7001,8 +7001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="14.5"/>
@@ -7300,8 +7300,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A36">
-    <sortCondition ref="A3:A36"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B36">
+    <sortCondition ref="A2:A36"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Añadida silicona para parabrisas
</commit_message>
<xml_diff>
--- a/clientes/files/TODITICO_CATÁLOGO.xlsx
+++ b/clientes/files/TODITICO_CATÁLOGO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trabajo\Catálogos Proformas\Este\330 Actual\Clientes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA941F34-1C99-4F83-A53E-2983E8987453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34995BAB-2601-4FE7-9E7B-587090CB6FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="621">
   <si>
     <t>DESCRIPCION</t>
   </si>
@@ -1953,6 +1953,9 @@
   </si>
   <si>
     <t>ARTICULACION DE LIMPIAPARABRISAS DE BOLA CHICA</t>
+  </si>
+  <si>
+    <t>SILICONA PARA PARABRISAS</t>
   </si>
 </sst>
 </file>
@@ -7421,10 +7424,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B39"/>
+      <selection activeCell="B37" sqref="B37:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="14.5"/>
@@ -7723,25 +7726,33 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>446</v>
+        <v>620</v>
       </c>
       <c r="B37" s="1">
-        <v>3960</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B38" s="1">
-        <v>3300</v>
+        <v>3960</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
+        <v>448</v>
+      </c>
+      <c r="B39" s="1">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
         <v>615</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B40" s="1">
         <v>4950</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update document with new products
</commit_message>
<xml_diff>
--- a/clientes/files/TODITICO_CATÁLOGO.xlsx
+++ b/clientes/files/TODITICO_CATÁLOGO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trabajo\Catálogos Proformas\Este\330 Actual - Cosas Nuevas\Clientes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B950B1-E164-4274-AFB0-70EEA4940C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E39BC5A-E948-4D72-B08B-4A59B90862CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="671" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAEWOO TICO" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="653">
   <si>
     <t>DESCRIPCION</t>
   </si>
@@ -1867,9 +1867,6 @@
     <t>ARTICULACION DE LIMPIAPARABRISAS DE BOLA CHICA</t>
   </si>
   <si>
-    <t>ANTENA CON LUZ</t>
-  </si>
-  <si>
     <t xml:space="preserve">CARGADOR PARA MOVILES </t>
   </si>
   <si>
@@ -1894,9 +1891,6 @@
     <t>TOPE DE PUERTA KIA C/U</t>
   </si>
   <si>
-    <t>VALVULAS DE LLANTAS JGO</t>
-  </si>
-  <si>
     <t>CINTA DEL TIMON PICANTO 2DA</t>
   </si>
   <si>
@@ -1991,6 +1985,15 @@
   </si>
   <si>
     <t>CILINDRO DE PUERTAS Y MALETERO JGO</t>
+  </si>
+  <si>
+    <t>TAPAS CÓNICAS DE VALVULAS DE LLANTAS JGO</t>
+  </si>
+  <si>
+    <t>ANTENA O ALETA DE TIBURÓN CON LUZ</t>
+  </si>
+  <si>
+    <t>CLIPS DE ACABADOS PLÁSTICOS DE PUERTA TIPO TRIÁNGULO C/U</t>
   </si>
 </sst>
 </file>
@@ -2103,7 +2106,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2194,6 +2197,11 @@
     <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2470,10 +2478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B312"/>
+  <dimension ref="A1:B313"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B312"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="14.5"/>
@@ -2627,8 +2635,8 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>610</v>
+      <c r="A19" s="34" t="s">
+        <v>651</v>
       </c>
       <c r="B19" s="1">
         <v>3300</v>
@@ -2748,7 +2756,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B34" s="1">
         <v>4950</v>
@@ -3196,7 +3204,7 @@
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B90" s="1">
         <v>4950</v>
@@ -3252,7 +3260,7 @@
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B97" s="1">
         <v>14850</v>
@@ -3268,7 +3276,7 @@
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B99" s="1">
         <v>8250</v>
@@ -3300,7 +3308,7 @@
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B103" s="1">
         <v>9900</v>
@@ -3308,135 +3316,135 @@
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>252</v>
+        <v>652</v>
       </c>
       <c r="B104" s="1">
-        <v>39600</v>
+        <v>82.5</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B105" s="1">
-        <v>9900</v>
+        <v>39600</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B106" s="1">
-        <v>19800</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>448</v>
+        <v>254</v>
       </c>
       <c r="B107" s="1">
-        <v>3300</v>
+        <v>19800</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>255</v>
+        <v>448</v>
       </c>
       <c r="B108" s="1">
-        <v>6600</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B109" s="1">
-        <v>4950</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B110" s="1">
-        <v>6600</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B111" s="1">
-        <v>19800</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B112" s="1">
-        <v>49500</v>
+        <v>19800</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B113" s="1">
-        <v>13200</v>
+        <v>49500</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>471</v>
+        <v>260</v>
       </c>
       <c r="B114" s="1">
-        <v>33000</v>
+        <v>13200</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>261</v>
+        <v>471</v>
       </c>
       <c r="B115" s="1">
-        <v>8250</v>
+        <v>33000</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B116" s="1">
-        <v>148500</v>
+        <v>8250</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B117" s="1">
-        <v>59400</v>
+        <v>148500</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>500</v>
+        <v>263</v>
       </c>
       <c r="B118" s="1">
-        <v>3300</v>
+        <v>59400</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B119" s="1">
-        <v>9900</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B120" s="1">
         <v>9900</v>
@@ -3444,135 +3452,135 @@
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>264</v>
+        <v>502</v>
       </c>
       <c r="B121" s="1">
-        <v>19800</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B122" s="1">
-        <v>39600</v>
+        <v>19800</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B123" s="1">
-        <v>8250</v>
+        <v>39600</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B124" s="1">
-        <v>26400</v>
+        <v>8250</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>459</v>
+        <v>268</v>
       </c>
       <c r="B125" s="1">
-        <v>82500</v>
+        <v>26400</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="4" t="s">
-        <v>15</v>
+        <v>459</v>
       </c>
       <c r="B126" s="1">
-        <v>39600</v>
+        <v>82500</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>269</v>
+        <v>15</v>
       </c>
       <c r="B127" s="1">
-        <v>6600</v>
+        <v>39600</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B128" s="1">
-        <v>4950</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>612</v>
+        <v>267</v>
       </c>
       <c r="B129" s="1">
-        <v>3300</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>270</v>
+        <v>611</v>
       </c>
       <c r="B130" s="1">
-        <v>16500</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B131" s="1">
-        <v>19800</v>
+        <v>16500</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B132" s="1">
-        <v>33000</v>
+        <v>19800</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>418</v>
+        <v>272</v>
       </c>
       <c r="B133" s="1">
-        <v>4950</v>
+        <v>33000</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>273</v>
+        <v>418</v>
       </c>
       <c r="B134" s="1">
-        <v>16500</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B135" s="1">
-        <v>23100</v>
+        <v>16500</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B136" s="1">
-        <v>3300</v>
+        <v>23100</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B137" s="1">
         <v>3300</v>
@@ -3580,7 +3588,7 @@
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B138" s="1">
         <v>3300</v>
@@ -3588,175 +3596,175 @@
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B139" s="1">
-        <v>9900</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B140" s="1">
-        <v>29700</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B141" s="1">
-        <v>16500</v>
+        <v>29700</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="B142" s="1">
-        <v>3300</v>
+        <v>16500</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B143" s="1">
-        <v>9900</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>507</v>
+        <v>279</v>
       </c>
       <c r="B144" s="1">
-        <v>6600</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>280</v>
+        <v>507</v>
       </c>
       <c r="B145" s="1">
-        <v>39600</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B146" s="1">
-        <v>4950</v>
+        <v>39600</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B147" s="1">
-        <v>23100</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B148" s="1">
-        <v>6600</v>
+        <v>23100</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>531</v>
+        <v>286</v>
       </c>
       <c r="B149" s="1">
-        <v>3300</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>287</v>
+        <v>531</v>
       </c>
       <c r="B150" s="1">
-        <v>1650</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B151" s="1">
-        <v>33000</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B152" s="1">
-        <v>19800</v>
+        <v>33000</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B153" s="1">
-        <v>9900</v>
+        <v>19800</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B154" s="1">
-        <v>33000</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B155" s="1">
-        <v>9900</v>
+        <v>33000</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B156" s="1">
-        <v>3300</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B157" s="1">
-        <v>4950</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B158" s="1">
-        <v>9900</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B159" s="1">
-        <v>3300</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>461</v>
+        <v>296</v>
       </c>
       <c r="B160" s="1">
         <v>3300</v>
@@ -3764,7 +3772,7 @@
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B161" s="1">
         <v>3300</v>
@@ -3772,159 +3780,159 @@
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>297</v>
+        <v>462</v>
       </c>
       <c r="B162" s="1">
-        <v>6600</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B163" s="1">
-        <v>660</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B164" s="1">
-        <v>6600</v>
+        <v>660</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B165" s="1">
-        <v>16500</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B166" s="1">
-        <v>13200</v>
+        <v>16500</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>508</v>
+        <v>301</v>
       </c>
       <c r="B167" s="1">
-        <v>49500</v>
+        <v>13200</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>302</v>
+        <v>508</v>
       </c>
       <c r="B168" s="1">
-        <v>29700</v>
+        <v>49500</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B169" s="1">
-        <v>3960</v>
+        <v>29700</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B170" s="1">
-        <v>4950</v>
+        <v>3960</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>511</v>
+        <v>304</v>
       </c>
       <c r="B171" s="1">
-        <v>132000</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>305</v>
+        <v>511</v>
       </c>
       <c r="B172" s="1">
-        <v>181500</v>
+        <v>132000</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B173" s="1">
-        <v>1980</v>
+        <v>181500</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B174" s="1">
-        <v>3300</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>449</v>
+        <v>307</v>
       </c>
       <c r="B175" s="1">
-        <v>6600</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>308</v>
+        <v>449</v>
       </c>
       <c r="B176" s="1">
-        <v>4950</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>450</v>
+        <v>308</v>
       </c>
       <c r="B177" s="1">
-        <v>1650</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>309</v>
+        <v>450</v>
       </c>
       <c r="B178" s="1">
-        <v>4950</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B179" s="1">
-        <v>23100</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B180" s="1">
-        <v>3300</v>
+        <v>23100</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B181" s="1">
         <v>3300</v>
@@ -3932,23 +3940,23 @@
     </row>
     <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B182" s="1">
-        <v>6600</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B183" s="1">
-        <v>3300</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B184" s="1">
         <v>3300</v>
@@ -3956,7 +3964,7 @@
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B185" s="1">
         <v>3300</v>
@@ -3964,31 +3972,31 @@
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>613</v>
+        <v>316</v>
       </c>
       <c r="B186" s="1">
-        <v>3960</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>317</v>
+        <v>612</v>
       </c>
       <c r="B187" s="1">
-        <v>16500</v>
+        <v>3960</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>514</v>
+        <v>317</v>
       </c>
       <c r="B188" s="1">
-        <v>1650</v>
+        <v>16500</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="B189" s="1">
         <v>1650</v>
@@ -3996,231 +4004,231 @@
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>318</v>
+        <v>509</v>
       </c>
       <c r="B190" s="1">
-        <v>9900</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B191" s="1">
-        <v>2310</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B192" s="1">
-        <v>92400</v>
+        <v>2310</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B193" s="1">
-        <v>49500</v>
+        <v>92400</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>634</v>
+        <v>321</v>
       </c>
       <c r="B194" s="1">
-        <v>21450</v>
+        <v>49500</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>451</v>
+        <v>632</v>
       </c>
       <c r="B195" s="1">
-        <v>26400</v>
+        <v>21450</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>322</v>
+        <v>451</v>
       </c>
       <c r="B196" s="1">
-        <v>9900</v>
+        <v>26400</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B197" s="1">
-        <v>49500</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B198" s="1">
-        <v>3300</v>
+        <v>49500</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>635</v>
+        <v>324</v>
       </c>
       <c r="B199" s="1">
-        <v>19800</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" t="s">
-        <v>325</v>
+        <v>633</v>
       </c>
       <c r="B200" s="1">
-        <v>3300</v>
+        <v>19800</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B201" s="1">
-        <v>6600</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B202" s="1">
-        <v>33000</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B203" s="1">
-        <v>39600</v>
+        <v>33000</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B204" s="1">
-        <v>99000</v>
+        <v>39600</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B205" s="1">
-        <v>52800</v>
+        <v>99000</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B206" s="1">
-        <v>36300</v>
+        <v>52800</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B207" s="1">
-        <v>52800</v>
+        <v>36300</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B208" s="1">
-        <v>9900</v>
+        <v>52800</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B209" s="1">
-        <v>56100</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B210" s="1">
-        <v>26400</v>
+        <v>56100</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B211" s="1">
-        <v>72600</v>
+        <v>26400</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B212" s="1">
-        <v>29700</v>
+        <v>72600</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B213" s="1">
-        <v>8250</v>
+        <v>29700</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B214" s="1">
-        <v>23100</v>
+        <v>8250</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B215" s="1">
-        <v>8250</v>
+        <v>23100</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B216" s="1">
-        <v>3300</v>
+        <v>8250</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217" t="s">
-        <v>512</v>
+        <v>341</v>
       </c>
       <c r="B217" s="1">
-        <v>6600</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B218" s="1">
         <v>6600</v>
@@ -4228,15 +4236,15 @@
     </row>
     <row r="219" spans="1:2">
       <c r="A219" t="s">
-        <v>342</v>
+        <v>513</v>
       </c>
       <c r="B219" s="1">
-        <v>9900</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B220" s="1">
         <v>9900</v>
@@ -4244,39 +4252,39 @@
     </row>
     <row r="221" spans="1:2">
       <c r="A221" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B221" s="1">
-        <v>19800</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222" t="s">
-        <v>453</v>
+        <v>344</v>
       </c>
       <c r="B222" s="1">
-        <v>13200</v>
+        <v>19800</v>
       </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223" t="s">
-        <v>345</v>
+        <v>453</v>
       </c>
       <c r="B223" s="1">
-        <v>9900</v>
+        <v>13200</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B224" s="1">
-        <v>6600</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B225" s="1">
         <v>6600</v>
@@ -4284,31 +4292,31 @@
     </row>
     <row r="226" spans="1:2">
       <c r="A226" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B226" s="1">
-        <v>49500</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B227" s="1">
-        <v>115500</v>
+        <v>49500</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B228" s="1">
-        <v>6600</v>
+        <v>115500</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B229" s="1">
         <v>6600</v>
@@ -4316,151 +4324,151 @@
     </row>
     <row r="230" spans="1:2">
       <c r="A230" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B230" s="1">
-        <v>4950</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B231" s="1">
-        <v>9900</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B232" s="1">
-        <v>4950</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B233" s="1">
-        <v>23100</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B234" s="1">
-        <v>13200</v>
+        <v>23100</v>
       </c>
     </row>
     <row r="235" spans="1:2">
       <c r="A235" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B235" s="1">
-        <v>33000</v>
+        <v>13200</v>
       </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B236" s="1">
-        <v>23100</v>
+        <v>33000</v>
       </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B237" s="1">
-        <v>4950</v>
+        <v>23100</v>
       </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B238" s="1">
-        <v>42900</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B239" s="1">
-        <v>66000</v>
+        <v>42900</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B240" s="1">
-        <v>9900</v>
+        <v>66000</v>
       </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B241" s="1">
-        <v>4950</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242" t="s">
-        <v>636</v>
+        <v>363</v>
       </c>
       <c r="B242" s="1">
-        <v>33000</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243" t="s">
-        <v>364</v>
+        <v>634</v>
       </c>
       <c r="B243" s="1">
-        <v>21450</v>
+        <v>33000</v>
       </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B244" s="1">
-        <v>31350</v>
+        <v>21450</v>
       </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B245" s="1">
-        <v>3300</v>
+        <v>31350</v>
       </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B246" s="1">
-        <v>6600</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B247" s="1">
-        <v>3300</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B248" s="1">
         <v>3300</v>
@@ -4468,7 +4476,7 @@
     </row>
     <row r="249" spans="1:2">
       <c r="A249" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B249" s="1">
         <v>3300</v>
@@ -4476,7 +4484,7 @@
     </row>
     <row r="250" spans="1:2">
       <c r="A250" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B250" s="1">
         <v>3300</v>
@@ -4484,15 +4492,15 @@
     </row>
     <row r="251" spans="1:2">
       <c r="A251" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B251" s="1">
-        <v>4950</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B252" s="1">
         <v>4950</v>
@@ -4500,7 +4508,7 @@
     </row>
     <row r="253" spans="1:2">
       <c r="A253" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B253" s="1">
         <v>4950</v>
@@ -4508,7 +4516,7 @@
     </row>
     <row r="254" spans="1:2">
       <c r="A254" t="s">
-        <v>454</v>
+        <v>374</v>
       </c>
       <c r="B254" s="1">
         <v>4950</v>
@@ -4516,167 +4524,167 @@
     </row>
     <row r="255" spans="1:2">
       <c r="A255" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B255" s="1">
-        <v>1980</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="256" spans="1:2">
       <c r="A256" t="s">
-        <v>375</v>
+        <v>455</v>
       </c>
       <c r="B256" s="1">
-        <v>3300</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="257" spans="1:2">
       <c r="A257" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B257" s="1">
-        <v>49500</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="258" spans="1:2">
       <c r="A258" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B258" s="1">
-        <v>59400</v>
+        <v>49500</v>
       </c>
     </row>
     <row r="259" spans="1:2">
       <c r="A259" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B259" s="1">
-        <v>29700</v>
+        <v>59400</v>
       </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B260" s="1">
-        <v>9900</v>
+        <v>29700</v>
       </c>
     </row>
     <row r="261" spans="1:2">
       <c r="A261" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B261" s="1">
-        <v>8250</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="262" spans="1:2">
       <c r="A262" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B262" s="1">
-        <v>1320</v>
+        <v>8250</v>
       </c>
     </row>
     <row r="263" spans="1:2">
       <c r="A263" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B263" s="1">
-        <v>24750</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="264" spans="1:2">
       <c r="A264" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B264" s="1">
-        <v>8250</v>
+        <v>24750</v>
       </c>
     </row>
     <row r="265" spans="1:2">
       <c r="A265" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B265" s="1">
-        <v>23100</v>
+        <v>8250</v>
       </c>
     </row>
     <row r="266" spans="1:2">
       <c r="A266" t="s">
-        <v>637</v>
+        <v>384</v>
       </c>
       <c r="B266" s="1">
-        <v>3960</v>
+        <v>23100</v>
       </c>
     </row>
     <row r="267" spans="1:2">
       <c r="A267" t="s">
-        <v>385</v>
+        <v>635</v>
       </c>
       <c r="B267" s="1">
-        <v>4950</v>
+        <v>3960</v>
       </c>
     </row>
     <row r="268" spans="1:2">
       <c r="A268" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B268" s="1">
-        <v>82500</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="269" spans="1:2">
       <c r="A269" t="s">
-        <v>445</v>
+        <v>386</v>
       </c>
       <c r="B269" s="1">
-        <v>181500</v>
+        <v>82500</v>
       </c>
     </row>
     <row r="270" spans="1:2">
       <c r="A270" t="s">
-        <v>387</v>
+        <v>445</v>
       </c>
       <c r="B270" s="1">
-        <v>8250</v>
+        <v>181500</v>
       </c>
     </row>
     <row r="271" spans="1:2">
       <c r="A271" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B271" s="1">
-        <v>3300</v>
+        <v>8250</v>
       </c>
     </row>
     <row r="272" spans="1:2">
       <c r="A272" t="s">
-        <v>638</v>
+        <v>388</v>
       </c>
       <c r="B272" s="1">
-        <v>6600</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273" t="s">
-        <v>389</v>
+        <v>636</v>
       </c>
       <c r="B273" s="1">
-        <v>3300</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="274" spans="1:2">
       <c r="A274" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B274" s="1">
-        <v>4950</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="275" spans="1:2">
       <c r="A275" t="s">
-        <v>639</v>
+        <v>390</v>
       </c>
       <c r="B275" s="1">
         <v>4950</v>
@@ -4684,39 +4692,39 @@
     </row>
     <row r="276" spans="1:2">
       <c r="A276" t="s">
-        <v>391</v>
+        <v>637</v>
       </c>
       <c r="B276" s="1">
-        <v>2310</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="277" spans="1:2">
       <c r="A277" t="s">
-        <v>392</v>
+        <v>650</v>
       </c>
       <c r="B277" s="1">
-        <v>16500</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="278" spans="1:2">
       <c r="A278" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B278" s="1">
-        <v>1650</v>
+        <v>2310</v>
       </c>
     </row>
     <row r="279" spans="1:2">
       <c r="A279" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B279" s="1">
-        <v>1650</v>
+        <v>16500</v>
       </c>
     </row>
     <row r="280" spans="1:2">
       <c r="A280" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B280" s="1">
         <v>1650</v>
@@ -4724,55 +4732,55 @@
     </row>
     <row r="281" spans="1:2">
       <c r="A281" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B281" s="1">
-        <v>2310</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="282" spans="1:2">
       <c r="A282" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B282" s="1">
-        <v>6600</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="283" spans="1:2">
       <c r="A283" t="s">
-        <v>439</v>
+        <v>396</v>
       </c>
       <c r="B283" s="1">
-        <v>3300</v>
+        <v>2310</v>
       </c>
     </row>
     <row r="284" spans="1:2">
       <c r="A284" t="s">
-        <v>605</v>
+        <v>397</v>
       </c>
       <c r="B284" s="1">
-        <v>4950</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="285" spans="1:2">
       <c r="A285" t="s">
-        <v>398</v>
+        <v>439</v>
       </c>
       <c r="B285" s="1">
-        <v>4950</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="286" spans="1:2">
       <c r="A286" t="s">
-        <v>616</v>
+        <v>605</v>
       </c>
       <c r="B286" s="1">
-        <v>8250</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="287" spans="1:2">
       <c r="A287" t="s">
-        <v>617</v>
+        <v>398</v>
       </c>
       <c r="B287" s="1">
         <v>4950</v>
@@ -4780,63 +4788,63 @@
     </row>
     <row r="288" spans="1:2">
       <c r="A288" t="s">
-        <v>399</v>
+        <v>615</v>
       </c>
       <c r="B288" s="1">
-        <v>1650</v>
+        <v>8250</v>
       </c>
     </row>
     <row r="289" spans="1:2">
       <c r="A289" t="s">
-        <v>400</v>
+        <v>616</v>
       </c>
       <c r="B289" s="1">
-        <v>2310</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="290" spans="1:2">
       <c r="A290" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B290" s="1">
-        <v>3300</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="291" spans="1:2">
       <c r="A291" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B291" s="1">
-        <v>660</v>
+        <v>2310</v>
       </c>
     </row>
     <row r="292" spans="1:2">
       <c r="A292" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B292" s="1">
-        <v>1650</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="293" spans="1:2">
       <c r="A293" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B293" s="1">
-        <v>990</v>
+        <v>660</v>
       </c>
     </row>
     <row r="294" spans="1:2">
       <c r="A294" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B294" s="1">
-        <v>1320</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="295" spans="1:2">
       <c r="A295" t="s">
-        <v>452</v>
+        <v>404</v>
       </c>
       <c r="B295" s="1">
         <v>990</v>
@@ -4844,103 +4852,103 @@
     </row>
     <row r="296" spans="1:2">
       <c r="A296" t="s">
-        <v>510</v>
+        <v>405</v>
       </c>
       <c r="B296" s="1">
-        <v>2310</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="297" spans="1:2">
       <c r="A297" t="s">
-        <v>406</v>
+        <v>452</v>
       </c>
       <c r="B297" s="1">
-        <v>660</v>
+        <v>990</v>
       </c>
     </row>
     <row r="298" spans="1:2">
       <c r="A298" t="s">
-        <v>532</v>
+        <v>510</v>
       </c>
       <c r="B298" s="1">
-        <v>59400</v>
+        <v>2310</v>
       </c>
     </row>
     <row r="299" spans="1:2">
       <c r="A299" t="s">
-        <v>515</v>
+        <v>406</v>
       </c>
       <c r="B299" s="1">
-        <v>3300</v>
+        <v>660</v>
       </c>
     </row>
     <row r="300" spans="1:2">
       <c r="A300" t="s">
-        <v>407</v>
+        <v>532</v>
       </c>
       <c r="B300" s="1">
-        <v>6600</v>
+        <v>59400</v>
       </c>
     </row>
     <row r="301" spans="1:2">
       <c r="A301" t="s">
-        <v>408</v>
+        <v>515</v>
       </c>
       <c r="B301" s="1">
-        <v>8250</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="302" spans="1:2">
       <c r="A302" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B302" s="1">
-        <v>14850</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="303" spans="1:2">
       <c r="A303" t="s">
+        <v>408</v>
+      </c>
+      <c r="B303" s="1">
+        <v>8250</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2">
+      <c r="A304" s="34" t="s">
+        <v>409</v>
+      </c>
+      <c r="B304" s="1">
+        <v>14850</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2">
+      <c r="A305" s="34" t="s">
         <v>410</v>
       </c>
-      <c r="B303" s="1">
+      <c r="B305" s="1">
         <v>4950</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2">
-      <c r="A304" t="s">
-        <v>619</v>
-      </c>
-      <c r="B304" s="1">
-        <v>3300</v>
-      </c>
-    </row>
-    <row r="305" spans="1:2">
-      <c r="A305" t="s">
-        <v>411</v>
-      </c>
-      <c r="B305" s="1">
-        <v>19800</v>
       </c>
     </row>
     <row r="306" spans="1:2">
       <c r="A306" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B306" s="1">
-        <v>33000</v>
+        <v>19800</v>
       </c>
     </row>
     <row r="307" spans="1:2">
       <c r="A307" t="s">
-        <v>516</v>
+        <v>412</v>
       </c>
       <c r="B307" s="1">
-        <v>4950</v>
+        <v>33000</v>
       </c>
     </row>
     <row r="308" spans="1:2">
       <c r="A308" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B308" s="1">
         <v>4950</v>
@@ -4948,33 +4956,41 @@
     </row>
     <row r="309" spans="1:2">
       <c r="A309" t="s">
-        <v>413</v>
+        <v>517</v>
       </c>
       <c r="B309" s="1">
-        <v>11550</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="310" spans="1:2">
       <c r="A310" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B310" s="1">
-        <v>3300</v>
+        <v>11550</v>
       </c>
     </row>
     <row r="311" spans="1:2">
       <c r="A311" t="s">
-        <v>498</v>
+        <v>414</v>
       </c>
       <c r="B311" s="1">
-        <v>1650</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="312" spans="1:2">
       <c r="A312" t="s">
+        <v>498</v>
+      </c>
+      <c r="B312" s="1">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2">
+      <c r="A313" t="s">
         <v>415</v>
       </c>
-      <c r="B312" s="1">
+      <c r="B313" s="1">
         <v>4950</v>
       </c>
     </row>
@@ -5023,7 +5039,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="7" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B4" s="1">
         <v>59400</v>
@@ -5039,15 +5055,15 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="7" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B6" s="1">
         <v>39600</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="5" t="s">
-        <v>610</v>
+      <c r="A7" s="36" t="s">
+        <v>651</v>
       </c>
       <c r="B7" s="1">
         <v>3300</v>
@@ -5295,7 +5311,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="12" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B38" s="1">
         <v>4950</v>
@@ -5423,7 +5439,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="6" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B54" s="1">
         <v>3300</v>
@@ -5447,7 +5463,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="15" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B57" s="1">
         <v>3300</v>
@@ -5471,7 +5487,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="5" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B60" s="1">
         <v>4950</v>
@@ -5575,7 +5591,7 @@
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="5" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B73" s="1">
         <v>3960</v>
@@ -5815,7 +5831,7 @@
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="5" t="s">
-        <v>614</v>
+        <v>650</v>
       </c>
       <c r="B103" s="1">
         <v>3300</v>
@@ -5823,31 +5839,31 @@
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="5" t="s">
-        <v>560</v>
+        <v>613</v>
       </c>
       <c r="B104" s="1">
-        <v>9900</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>439</v>
+        <v>560</v>
       </c>
       <c r="B105" s="1">
-        <v>3300</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>605</v>
+        <v>439</v>
       </c>
       <c r="B106" s="1">
-        <v>4950</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>482</v>
+        <v>605</v>
       </c>
       <c r="B107" s="1">
         <v>4950</v>
@@ -5855,31 +5871,31 @@
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>616</v>
+        <v>482</v>
       </c>
       <c r="B108" s="1">
-        <v>8250</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B109" s="1">
-        <v>4950</v>
+        <v>8250</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
+        <v>616</v>
+      </c>
+      <c r="B110" s="1">
+        <v>4950</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="34" t="s">
         <v>475</v>
-      </c>
-      <c r="B110" s="1">
-        <v>3300</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="A111" t="s">
-        <v>619</v>
       </c>
       <c r="B111" s="1">
         <v>3300</v>
@@ -5900,10 +5916,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B207"/>
+  <dimension ref="A1:B206"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A2" sqref="A2:B206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="14.5"/>
@@ -5962,7 +5978,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="22" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B7" s="1">
         <v>59400</v>
@@ -5985,8 +6001,8 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="4" t="s">
-        <v>610</v>
+      <c r="A10" s="34" t="s">
+        <v>651</v>
       </c>
       <c r="B10" s="1">
         <v>3300</v>
@@ -6258,7 +6274,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B44" s="1">
         <v>33000</v>
@@ -6266,7 +6282,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="4" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B45" s="1">
         <v>24750</v>
@@ -6282,7 +6298,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="4" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B47" s="1">
         <v>4950</v>
@@ -6314,7 +6330,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="4" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B51" s="1">
         <v>9900</v>
@@ -6618,7 +6634,7 @@
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B89" s="1">
         <v>3300</v>
@@ -6658,7 +6674,7 @@
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="4" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B94" s="1">
         <v>3300</v>
@@ -6674,7 +6690,7 @@
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="4" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B96" s="1">
         <v>6600</v>
@@ -6682,7 +6698,7 @@
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="4" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B97" s="1">
         <v>9900</v>
@@ -6714,7 +6730,7 @@
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="27" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B101" s="1">
         <v>4950</v>
@@ -6722,7 +6738,7 @@
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="4" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B102" s="1">
         <v>6600</v>
@@ -6794,7 +6810,7 @@
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="4" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B111" s="1">
         <v>46200</v>
@@ -6906,7 +6922,7 @@
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B125" s="1">
         <v>3960</v>
@@ -7026,7 +7042,7 @@
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="4" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B140" s="1">
         <v>66000</v>
@@ -7090,7 +7106,7 @@
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="4" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B148" s="1">
         <v>11550</v>
@@ -7450,7 +7466,7 @@
     </row>
     <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>615</v>
+        <v>650</v>
       </c>
       <c r="B193" s="1">
         <v>3300</v>
@@ -7458,34 +7474,34 @@
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>128</v>
+        <v>614</v>
       </c>
       <c r="B194" s="1">
-        <v>9900</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>439</v>
+        <v>128</v>
       </c>
       <c r="B195" s="1">
-        <v>3300</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>605</v>
+        <v>439</v>
       </c>
       <c r="B196" s="1">
-        <v>4950</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>630</v>
+        <v>605</v>
       </c>
       <c r="B197" s="1">
-        <v>6600</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -7493,44 +7509,44 @@
         <v>628</v>
       </c>
       <c r="B198" s="1">
-        <v>9900</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>616</v>
+        <v>626</v>
       </c>
       <c r="B199" s="1">
-        <v>8250</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B200" s="1">
-        <v>4950</v>
+        <v>8250</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B201" s="1">
-        <v>1650</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" t="s">
+        <v>617</v>
+      </c>
+      <c r="B202" s="1">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2">
+      <c r="A203" s="34" t="s">
         <v>486</v>
-      </c>
-      <c r="B202" s="1">
-        <v>3300</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2">
-      <c r="A203" t="s">
-        <v>619</v>
       </c>
       <c r="B203" s="1">
         <v>3300</v>
@@ -7557,14 +7573,6 @@
         <v>167</v>
       </c>
       <c r="B206" s="1">
-        <v>13200</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2">
-      <c r="A207" t="s">
-        <v>167</v>
-      </c>
-      <c r="B207" s="1">
         <v>13200</v>
       </c>
     </row>
@@ -7595,8 +7603,8 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="32" t="s">
-        <v>610</v>
+      <c r="A2" s="35" t="s">
+        <v>651</v>
       </c>
       <c r="B2" s="1">
         <v>3300</v>
@@ -7604,7 +7612,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="32" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B3" s="1">
         <v>36300</v>
@@ -7644,7 +7652,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="32" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B8" s="1">
         <v>4950</v>
@@ -7684,7 +7692,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="32" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B13" s="1">
         <v>3300</v>
@@ -7708,7 +7716,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="32" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B16" s="1">
         <v>29700</v>
@@ -7716,7 +7724,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="32" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B17" s="1">
         <v>29700</v>
@@ -7780,7 +7788,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="32" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B25" s="1">
         <v>3960</v>
@@ -7820,71 +7828,71 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>607</v>
+        <v>650</v>
       </c>
       <c r="B30">
-        <v>23100</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B31">
-        <v>9900</v>
+        <v>23100</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>439</v>
+        <v>608</v>
       </c>
       <c r="B32">
-        <v>3300</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>605</v>
+        <v>439</v>
       </c>
       <c r="B33">
-        <v>4950</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>616</v>
+        <v>605</v>
       </c>
       <c r="B34">
-        <v>8250</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B35">
-        <v>4950</v>
+        <v>8250</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>596</v>
+        <v>616</v>
       </c>
       <c r="B36">
-        <v>3300</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
+        <v>596</v>
+      </c>
+      <c r="B37">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="34" t="s">
         <v>597</v>
-      </c>
-      <c r="B37">
-        <v>3300</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
-        <v>619</v>
       </c>
       <c r="B38">
         <v>3300</v>
@@ -7907,8 +7915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="14.5"/>
@@ -8006,8 +8014,8 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>610</v>
+      <c r="A12" s="34" t="s">
+        <v>651</v>
       </c>
       <c r="B12" s="1">
         <v>3300</v>
@@ -8031,7 +8039,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B15" s="1">
         <v>36300</v>
@@ -8071,7 +8079,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B20" s="1">
         <v>4950</v>
@@ -8087,7 +8095,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B22" s="1">
         <v>3300</v>
@@ -8143,7 +8151,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B29" s="1">
         <v>29700</v>
@@ -8151,7 +8159,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B30" s="1">
         <v>29700</v>
@@ -8215,7 +8223,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B38" s="1">
         <v>3960</v>
@@ -8263,7 +8271,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B44" s="1">
         <v>4950</v>
@@ -8279,7 +8287,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>614</v>
+        <v>650</v>
       </c>
       <c r="B46" s="1">
         <v>3300</v>
@@ -8287,7 +8295,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B47" s="1">
         <v>3300</v>
@@ -8295,7 +8303,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>439</v>
+        <v>614</v>
       </c>
       <c r="B48" s="1">
         <v>3300</v>
@@ -8303,42 +8311,42 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>605</v>
+        <v>439</v>
       </c>
       <c r="B49" s="1">
-        <v>4950</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>616</v>
+        <v>605</v>
       </c>
       <c r="B50" s="1">
-        <v>8250</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B51" s="1">
-        <v>4950</v>
+        <v>8250</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B52" s="1">
+        <v>4950</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="34" t="s">
+        <v>617</v>
+      </c>
+      <c r="B53" s="1">
         <v>1650</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
-        <v>619</v>
-      </c>
-      <c r="B53" s="1">
-        <v>3300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update documents with new products
</commit_message>
<xml_diff>
--- a/clientes/files/TODITICO_CATÁLOGO.xlsx
+++ b/clientes/files/TODITICO_CATÁLOGO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trabajo\Catálogos Proformas\Este\370 Actual\Clientes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41BA524-7B0A-42FA-9184-A31D3D014E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A38164E-0489-4A85-8996-DDD8E411B147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="671" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="671" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAEWOO TICO" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="702">
   <si>
     <t>DESCRIPCION</t>
   </si>
@@ -2130,10 +2130,17 @@
     <t>SEGUROS ANTIRROBOS</t>
   </si>
   <si>
-    <t>RADIADOR MECANICO ATOS</t>
-  </si>
-  <si>
     <t>PARABRISAS ATOS (97-03)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RADIADOR MECANICO ATOS
+</t>
+  </si>
+  <si>
+    <t>BATERIAS 110 Ah</t>
+  </si>
+  <si>
+    <t>BATERIAS 120 Ah</t>
   </si>
 </sst>
 </file>
@@ -2628,8 +2635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B337"/>
   <sheetViews>
-    <sheetView topLeftCell="A321" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B337"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="14.5"/>
@@ -5343,8 +5350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="14.5"/>
@@ -6027,7 +6034,7 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B85" s="1">
         <v>129500</v>
@@ -6113,9 +6120,9 @@
         <v>55500</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" ht="29">
       <c r="A96" s="11" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B96" s="1">
         <v>48100</v>
@@ -6417,7 +6424,7 @@
         <v>141</v>
       </c>
       <c r="B12" s="1">
-        <v>12950</v>
+        <v>14800</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6425,7 +6432,7 @@
         <v>142</v>
       </c>
       <c r="B13" s="1">
-        <v>12950</v>
+        <v>14800</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -7569,7 +7576,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="1">
-        <v>12950</v>
+        <v>14800</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -7577,7 +7584,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="1">
-        <v>12950</v>
+        <v>14800</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -8501,10 +8508,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:B48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="14.5"/>
@@ -8619,63 +8626,63 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>453</v>
+        <v>700</v>
       </c>
       <c r="B14" s="1">
-        <v>29600</v>
+        <v>77700</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>172</v>
+        <v>701</v>
       </c>
       <c r="B15" s="1">
-        <v>37000</v>
+        <v>90650</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>689</v>
+        <v>453</v>
       </c>
       <c r="B16" s="1">
-        <v>37000</v>
+        <v>29600</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>619</v>
+        <v>172</v>
       </c>
       <c r="B17" s="1">
-        <v>40700</v>
+        <v>37000</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B18" s="1">
-        <v>44400</v>
+        <v>37000</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>426</v>
+        <v>619</v>
       </c>
       <c r="B19" s="1">
-        <v>370</v>
+        <v>40700</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>427</v>
+        <v>690</v>
       </c>
       <c r="B20" s="1">
-        <v>370</v>
+        <v>44400</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="B21" s="1">
         <v>370</v>
@@ -8683,23 +8690,23 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>452</v>
+        <v>427</v>
       </c>
       <c r="B22" s="1">
-        <v>3700</v>
+        <v>370</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>589</v>
+        <v>421</v>
       </c>
       <c r="B23" s="1">
-        <v>5550</v>
+        <v>370</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>409</v>
+        <v>452</v>
       </c>
       <c r="B24" s="1">
         <v>3700</v>
@@ -8707,15 +8714,15 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B25" s="1">
-        <v>3700</v>
+        <v>5550</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="B26" s="1">
         <v>3700</v>
@@ -8723,47 +8730,47 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>272</v>
+        <v>590</v>
       </c>
       <c r="B27" s="1">
-        <v>11100</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>448</v>
+        <v>423</v>
       </c>
       <c r="B28" s="1">
-        <v>1850</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>424</v>
+        <v>272</v>
       </c>
       <c r="B29" s="1">
-        <v>25900</v>
+        <v>11100</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>691</v>
+        <v>448</v>
       </c>
       <c r="B30" s="1">
-        <v>25900</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>693</v>
+        <v>424</v>
       </c>
       <c r="B31" s="1">
-        <v>29600</v>
+        <v>25900</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>173</v>
+        <v>691</v>
       </c>
       <c r="B32" s="1">
         <v>25900</v>
@@ -8771,7 +8778,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>447</v>
+        <v>693</v>
       </c>
       <c r="B33" s="1">
         <v>29600</v>
@@ -8779,39 +8786,39 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>620</v>
+        <v>173</v>
       </c>
       <c r="B34" s="1">
-        <v>33300</v>
+        <v>25900</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>621</v>
+        <v>447</v>
       </c>
       <c r="B35" s="1">
-        <v>33300</v>
+        <v>29600</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>512</v>
+        <v>620</v>
       </c>
       <c r="B36" s="1">
-        <v>3700</v>
+        <v>33300</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>410</v>
+        <v>621</v>
       </c>
       <c r="B37" s="1">
-        <v>4440</v>
+        <v>33300</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>411</v>
+        <v>512</v>
       </c>
       <c r="B38" s="1">
         <v>3700</v>
@@ -8819,15 +8826,15 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B39" s="1">
-        <v>5550</v>
+        <v>4440</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>680</v>
+        <v>411</v>
       </c>
       <c r="B40" s="1">
         <v>3700</v>
@@ -8835,31 +8842,31 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B41" s="1">
-        <v>4440</v>
+        <v>5550</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>414</v>
+        <v>680</v>
       </c>
       <c r="B42" s="1">
-        <v>4440</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B43" s="1">
-        <v>3700</v>
+        <v>4440</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>591</v>
+        <v>414</v>
       </c>
       <c r="B44" s="1">
         <v>4440</v>
@@ -8867,55 +8874,55 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>681</v>
+        <v>415</v>
       </c>
       <c r="B45" s="1">
-        <v>4440</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>578</v>
+        <v>591</v>
       </c>
       <c r="B46" s="1">
-        <v>6660</v>
+        <v>4440</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>416</v>
+        <v>681</v>
       </c>
       <c r="B47" s="1">
-        <v>7400</v>
+        <v>4440</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>697</v>
+        <v>578</v>
       </c>
       <c r="B48" s="1">
-        <v>5550</v>
+        <v>6660</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B49" s="1">
-        <v>4440</v>
+        <v>7400</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>418</v>
+        <v>697</v>
       </c>
       <c r="B50" s="1">
-        <v>2590</v>
+        <v>5550</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B51" s="1">
         <v>4440</v>
@@ -8923,15 +8930,15 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>622</v>
+        <v>418</v>
       </c>
       <c r="B52" s="1">
-        <v>5550</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B53" s="1">
         <v>4440</v>
@@ -8939,23 +8946,23 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="4" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="B54" s="1">
-        <v>3700</v>
+        <v>5550</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>592</v>
+        <v>420</v>
       </c>
       <c r="B55" s="1">
-        <v>3700</v>
+        <v>4440</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>593</v>
+        <v>628</v>
       </c>
       <c r="B56" s="1">
         <v>3700</v>
@@ -8963,47 +8970,47 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>686</v>
+        <v>592</v>
       </c>
       <c r="B57" s="1">
-        <v>2590</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>687</v>
+        <v>593</v>
       </c>
       <c r="B58" s="1">
-        <v>1850</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>422</v>
+        <v>686</v>
       </c>
       <c r="B59" s="1">
-        <v>3700</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>584</v>
+        <v>687</v>
       </c>
       <c r="B60" s="1">
-        <v>5550</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>594</v>
+        <v>422</v>
       </c>
       <c r="B61" s="1">
-        <v>9250</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>595</v>
+        <v>584</v>
       </c>
       <c r="B62" s="1">
         <v>5550</v>
@@ -9011,9 +9018,25 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
+        <v>594</v>
+      </c>
+      <c r="B63" s="1">
+        <v>9250</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>595</v>
+      </c>
+      <c r="B64" s="1">
+        <v>5550</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
         <v>596</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B65" s="1">
         <v>1850</v>
       </c>
     </row>

</xml_diff>